<commit_message>
Earth radius and G_constant
Fixed inconsistencies in constants
</commit_message>
<xml_diff>
--- a/AllEventData.xlsx
+++ b/AllEventData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\GitHub\strewnlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4913A4C7-DA19-45AD-AA22-9B8AA728A3BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D35623C-EA92-452E-85C7-AD9F17CB9952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C46C341C-A654-450D-9491-A8F495B2F4ED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C46C341C-A654-450D-9491-A8F495B2F4ED}"/>
   </bookViews>
   <sheets>
     <sheet name="AllEventData" sheetId="1" r:id="rId1"/>
@@ -8794,10 +8794,10 @@
   <dimension ref="A1:BI161"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="AK6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="AE168" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AS8" sqref="AS8"/>
+      <selection pane="bottomRight" activeCell="AI3" sqref="AI3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Database import validation and standardization
</commit_message>
<xml_diff>
--- a/AllEventData.xlsx
+++ b/AllEventData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\GitHub\strewnlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA18B516-AEE0-456C-846B-EAD640478A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53C5A40-C542-4BC3-8819-EFA0D4BD9F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C46C341C-A654-450D-9491-A8F495B2F4ED}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{C46C341C-A654-450D-9491-A8F495B2F4ED}"/>
   </bookViews>
   <sheets>
     <sheet name="AllEventData" sheetId="1" r:id="rId1"/>
@@ -8794,10 +8794,10 @@
   <dimension ref="A1:BI161"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="AA6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="E159" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AE4" sqref="AE4"/>
+      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Database import improvements in progress
</commit_message>
<xml_diff>
--- a/AllEventData.xlsx
+++ b/AllEventData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\GitHub\strewnlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53C5A40-C542-4BC3-8819-EFA0D4BD9F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9064A1B2-AB90-4272-890B-06D7266BDBDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{C46C341C-A654-450D-9491-A8F495B2F4ED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C46C341C-A654-450D-9491-A8F495B2F4ED}"/>
   </bookViews>
   <sheets>
     <sheet name="AllEventData" sheetId="1" r:id="rId1"/>
@@ -8794,10 +8794,10 @@
   <dimension ref="A1:BI161"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="E159" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="I29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomRight" activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14241,10 +14241,10 @@
         <f>F36+G36/24</f>
         <v>4584.791666666667</v>
       </c>
+      <c r="O36" s="3">
+        <v>34.9</v>
+      </c>
       <c r="P36" s="3">
-        <v>34.9</v>
-      </c>
-      <c r="Q36" s="3">
         <v>-110.1833</v>
       </c>
       <c r="W36" s="9" t="s">
@@ -14310,10 +14310,10 @@
         <f>F37+G37/24</f>
         <v>29558.322916666668</v>
       </c>
+      <c r="O37" s="3">
+        <v>15</v>
+      </c>
       <c r="P37" s="3">
-        <v>15</v>
-      </c>
-      <c r="Q37" s="3">
         <v>48.3</v>
       </c>
       <c r="W37" s="9" t="s">
@@ -39528,8 +39528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020F006F-09CB-4518-A6A0-B4628B5EF033}">
   <dimension ref="A1:D250"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="A233" sqref="A233:XFD233"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Database Improvements, solar elevation
</commit_message>
<xml_diff>
--- a/AllEventData.xlsx
+++ b/AllEventData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\GitHub\strewnlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCD35BC-10A9-402F-BC67-2DE4ACB44B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6386739F-967A-4102-B73A-261D9686215C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C46C341C-A654-450D-9491-A8F495B2F4ED}"/>
   </bookViews>
@@ -130,7 +130,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2859" uniqueCount="1607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2894" uniqueCount="1620">
   <si>
     <t>UTC Date and Time</t>
   </si>
@@ -4952,6 +4952,45 @@
   </si>
   <si>
     <t>vz</t>
+  </si>
+  <si>
+    <t>Bin</t>
+  </si>
+  <si>
+    <t>More</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Beira</t>
+  </si>
+  <si>
+    <t>Sofala</t>
+  </si>
+  <si>
+    <t>Toledo</t>
+  </si>
+  <si>
+    <t>https://www.caha.es/meteors-and-fireballs/14651-bright-fireball-above-madrid-and-toledo-provinces-on-the-second-of-april</t>
+  </si>
+  <si>
+    <t>Kryspin Kmieciak</t>
+  </si>
+  <si>
+    <t>Waite</t>
+  </si>
+  <si>
+    <t>Maine</t>
+  </si>
+  <si>
+    <t>Elmshorn</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Vincent Haberer</t>
   </si>
 </sst>
 </file>
@@ -4966,7 +5005,7 @@
     <numFmt numFmtId="168" formatCode="0.0"/>
     <numFmt numFmtId="169" formatCode="0.000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5067,6 +5106,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -5113,7 +5160,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -5207,6 +5254,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -5218,7 +5285,7 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -5362,6 +5429,10 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="169" fontId="3" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -8666,13 +8737,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{332638A7-5364-4539-88F3-B010BD503402}">
-  <dimension ref="A1:BI176"/>
+  <dimension ref="A1:BI180"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="M9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C172" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
+      <selection pane="bottomRight" activeCell="A181" sqref="A181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32665,7 +32736,7 @@
         <v>8</v>
       </c>
       <c r="H153" s="4">
-        <f t="shared" ref="H153:H176" si="10">F153+G153/24</f>
+        <f t="shared" ref="H153:H180" si="10">F153+G153/24</f>
         <v>44924.61954861111</v>
       </c>
       <c r="I153" s="3">
@@ -36250,6 +36321,753 @@
       </c>
       <c r="BI176" s="40">
         <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A177" s="6">
+        <v>176</v>
+      </c>
+      <c r="B177" s="6" t="s">
+        <v>853</v>
+      </c>
+      <c r="C177" s="6" t="s">
+        <v>1610</v>
+      </c>
+      <c r="D177" s="6" t="s">
+        <v>1611</v>
+      </c>
+      <c r="E177" s="6" t="s">
+        <v>853</v>
+      </c>
+      <c r="F177" s="17">
+        <v>45031.348622685182</v>
+      </c>
+      <c r="G177" s="21">
+        <v>2</v>
+      </c>
+      <c r="H177" s="4">
+        <f t="shared" si="10"/>
+        <v>45031.431956018518</v>
+      </c>
+      <c r="I177" s="3">
+        <v>178054</v>
+      </c>
+      <c r="J177" s="3">
+        <v>17210</v>
+      </c>
+      <c r="K177" s="3">
+        <f t="shared" ref="K177:K180" si="13">I177*J177^2/2/4.184/10^12</f>
+        <v>6.3021945197657745</v>
+      </c>
+      <c r="L177" s="3">
+        <v>294.10000000000002</v>
+      </c>
+      <c r="M177" s="3">
+        <v>54.8</v>
+      </c>
+      <c r="O177" s="3">
+        <v>-20.100000000000001</v>
+      </c>
+      <c r="P177" s="3">
+        <v>36</v>
+      </c>
+      <c r="Q177" s="3">
+        <v>41400</v>
+      </c>
+      <c r="R177" s="3">
+        <v>41400</v>
+      </c>
+      <c r="S177" s="3">
+        <v>5000</v>
+      </c>
+      <c r="T177" s="3">
+        <v>54.8</v>
+      </c>
+      <c r="U177" s="3">
+        <v>0</v>
+      </c>
+      <c r="V177" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="W177" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="X177" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y177" s="3">
+        <v>60000</v>
+      </c>
+      <c r="Z177" s="3">
+        <v>60000</v>
+      </c>
+      <c r="AA177" s="5">
+        <v>500</v>
+      </c>
+      <c r="AB177" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="AC177" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="AD177" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="AE177" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="AF177" s="5">
+        <v>500</v>
+      </c>
+      <c r="AG177" s="5">
+        <v>-1.5</v>
+      </c>
+      <c r="AH177" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="AI177" s="45">
+        <v>0</v>
+      </c>
+      <c r="AJ177" s="45">
+        <v>0</v>
+      </c>
+      <c r="AK177" s="45">
+        <v>0</v>
+      </c>
+      <c r="AL177" s="23">
+        <v>0</v>
+      </c>
+      <c r="AM177" s="23">
+        <v>0</v>
+      </c>
+      <c r="AN177" s="23">
+        <v>0</v>
+      </c>
+      <c r="AO177" s="23">
+        <v>0</v>
+      </c>
+      <c r="AP177" s="23">
+        <v>0</v>
+      </c>
+      <c r="AQ177" s="23">
+        <v>0</v>
+      </c>
+      <c r="AR177" s="25">
+        <v>0</v>
+      </c>
+      <c r="AS177" s="54">
+        <v>0</v>
+      </c>
+      <c r="AT177" s="52">
+        <v>0</v>
+      </c>
+      <c r="AU177" s="52">
+        <v>0</v>
+      </c>
+      <c r="AV177" s="52">
+        <v>0</v>
+      </c>
+      <c r="AW177" s="38">
+        <v>0</v>
+      </c>
+      <c r="AX177" s="38">
+        <v>4</v>
+      </c>
+      <c r="AY177" s="38">
+        <v>0</v>
+      </c>
+      <c r="AZ177" s="38">
+        <v>0</v>
+      </c>
+      <c r="BA177" s="38">
+        <v>0</v>
+      </c>
+      <c r="BB177" s="38">
+        <v>0</v>
+      </c>
+      <c r="BC177" s="38">
+        <v>4</v>
+      </c>
+      <c r="BD177" s="38">
+        <v>0</v>
+      </c>
+      <c r="BE177" s="38">
+        <v>0</v>
+      </c>
+      <c r="BF177" s="38">
+        <v>0</v>
+      </c>
+      <c r="BG177" s="40">
+        <v>2</v>
+      </c>
+      <c r="BH177" s="40" t="s">
+        <v>1416</v>
+      </c>
+      <c r="BI177" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A178" s="6">
+        <v>177</v>
+      </c>
+      <c r="B178" s="6" t="s">
+        <v>1612</v>
+      </c>
+      <c r="C178" s="6" t="s">
+        <v>1612</v>
+      </c>
+      <c r="D178" s="6" t="s">
+        <v>1612</v>
+      </c>
+      <c r="E178" s="6" t="s">
+        <v>1025</v>
+      </c>
+      <c r="F178" s="17">
+        <v>45018.811666666668</v>
+      </c>
+      <c r="G178" s="21">
+        <v>2</v>
+      </c>
+      <c r="H178" s="4">
+        <f t="shared" si="10"/>
+        <v>45018.895000000004</v>
+      </c>
+      <c r="I178" s="3">
+        <v>50</v>
+      </c>
+      <c r="J178" s="3">
+        <v>13610</v>
+      </c>
+      <c r="K178" s="3">
+        <f t="shared" si="13"/>
+        <v>1.10678836042065E-3</v>
+      </c>
+      <c r="L178" s="3">
+        <v>208.24</v>
+      </c>
+      <c r="M178" s="3">
+        <v>37.25</v>
+      </c>
+      <c r="N178" s="3" t="s">
+        <v>1334</v>
+      </c>
+      <c r="O178" s="3">
+        <v>39.803229999999999</v>
+      </c>
+      <c r="P178" s="3">
+        <v>-4.05924</v>
+      </c>
+      <c r="Q178" s="3">
+        <v>24000</v>
+      </c>
+      <c r="R178" s="3">
+        <v>24000</v>
+      </c>
+      <c r="S178" s="3">
+        <v>5000</v>
+      </c>
+      <c r="T178" s="3">
+        <f>M178</f>
+        <v>37.25</v>
+      </c>
+      <c r="U178" s="3">
+        <v>24000</v>
+      </c>
+      <c r="V178" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="W178" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="X178" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y178" s="3">
+        <v>60000</v>
+      </c>
+      <c r="Z178" s="3">
+        <v>60000</v>
+      </c>
+      <c r="AA178" s="5">
+        <v>500</v>
+      </c>
+      <c r="AB178" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="AC178" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="AD178" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="AE178" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="AF178" s="5">
+        <v>500</v>
+      </c>
+      <c r="AG178" s="5">
+        <v>-1.5</v>
+      </c>
+      <c r="AH178" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="AI178" s="45">
+        <v>0</v>
+      </c>
+      <c r="AJ178" s="45">
+        <v>0</v>
+      </c>
+      <c r="AK178" s="45">
+        <v>0</v>
+      </c>
+      <c r="AL178" s="23">
+        <v>0</v>
+      </c>
+      <c r="AM178" s="23">
+        <v>0</v>
+      </c>
+      <c r="AN178" s="23">
+        <v>0</v>
+      </c>
+      <c r="AO178" s="23">
+        <v>0</v>
+      </c>
+      <c r="AP178" s="23">
+        <v>0</v>
+      </c>
+      <c r="AQ178" s="23">
+        <v>0</v>
+      </c>
+      <c r="AR178" s="25">
+        <v>0</v>
+      </c>
+      <c r="AS178" s="54">
+        <v>0</v>
+      </c>
+      <c r="AT178" s="52">
+        <v>0</v>
+      </c>
+      <c r="AU178" s="52">
+        <v>0</v>
+      </c>
+      <c r="AV178" s="52">
+        <v>0</v>
+      </c>
+      <c r="AW178" s="38">
+        <v>0</v>
+      </c>
+      <c r="AX178" s="38">
+        <v>140</v>
+      </c>
+      <c r="AY178" s="38">
+        <v>0</v>
+      </c>
+      <c r="AZ178" s="38">
+        <v>0</v>
+      </c>
+      <c r="BA178" s="38">
+        <v>0</v>
+      </c>
+      <c r="BB178" s="38">
+        <v>0</v>
+      </c>
+      <c r="BC178" s="38">
+        <v>140</v>
+      </c>
+      <c r="BD178" s="38">
+        <v>0</v>
+      </c>
+      <c r="BE178" s="38">
+        <v>0</v>
+      </c>
+      <c r="BF178" s="38">
+        <v>0</v>
+      </c>
+      <c r="BG178" s="40">
+        <v>2</v>
+      </c>
+      <c r="BH178" s="40" t="s">
+        <v>1614</v>
+      </c>
+      <c r="BI178" s="40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A179" s="6">
+        <v>178</v>
+      </c>
+      <c r="B179" s="6" t="s">
+        <v>1615</v>
+      </c>
+      <c r="C179" s="6" t="s">
+        <v>1615</v>
+      </c>
+      <c r="D179" s="6" t="s">
+        <v>1616</v>
+      </c>
+      <c r="E179" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F179" s="17">
+        <v>45024.661458333336</v>
+      </c>
+      <c r="G179" s="21">
+        <v>-4</v>
+      </c>
+      <c r="H179" s="4">
+        <f t="shared" si="10"/>
+        <v>45024.494791666672</v>
+      </c>
+      <c r="I179" s="3">
+        <v>400</v>
+      </c>
+      <c r="J179" s="3">
+        <v>17000</v>
+      </c>
+      <c r="K179" s="3">
+        <f t="shared" si="13"/>
+        <v>1.381453154875717E-2</v>
+      </c>
+      <c r="L179" s="3">
+        <v>196</v>
+      </c>
+      <c r="M179" s="3">
+        <v>45</v>
+      </c>
+      <c r="N179" s="3" t="s">
+        <v>1334</v>
+      </c>
+      <c r="O179" s="3">
+        <v>45.390799999999999</v>
+      </c>
+      <c r="P179" s="3">
+        <v>-67.544799999999995</v>
+      </c>
+      <c r="Q179" s="3">
+        <v>16000</v>
+      </c>
+      <c r="R179" s="3">
+        <v>16000</v>
+      </c>
+      <c r="S179" s="3">
+        <v>5000</v>
+      </c>
+      <c r="T179" s="3">
+        <f>M179</f>
+        <v>45</v>
+      </c>
+      <c r="U179" s="3">
+        <v>12000</v>
+      </c>
+      <c r="V179" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="W179" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="X179" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y179" s="3">
+        <v>60000</v>
+      </c>
+      <c r="Z179" s="3">
+        <v>60000</v>
+      </c>
+      <c r="AA179" s="5">
+        <v>5000</v>
+      </c>
+      <c r="AB179" s="5">
+        <v>10</v>
+      </c>
+      <c r="AC179" s="5">
+        <v>10</v>
+      </c>
+      <c r="AD179" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="AE179" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="AF179" s="5">
+        <v>4000</v>
+      </c>
+      <c r="AG179" s="5">
+        <v>-1.5</v>
+      </c>
+      <c r="AH179" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="AI179" s="45">
+        <v>0</v>
+      </c>
+      <c r="AJ179" s="45">
+        <v>0</v>
+      </c>
+      <c r="AK179" s="45">
+        <v>0</v>
+      </c>
+      <c r="AL179" s="23">
+        <v>0</v>
+      </c>
+      <c r="AM179" s="23">
+        <v>0</v>
+      </c>
+      <c r="AN179" s="23">
+        <v>0</v>
+      </c>
+      <c r="AO179" s="23">
+        <v>0</v>
+      </c>
+      <c r="AP179" s="23">
+        <v>0</v>
+      </c>
+      <c r="AQ179" s="23">
+        <v>0</v>
+      </c>
+      <c r="AR179" s="25">
+        <v>0</v>
+      </c>
+      <c r="AS179" s="54">
+        <v>0</v>
+      </c>
+      <c r="AT179" s="52">
+        <v>0</v>
+      </c>
+      <c r="AU179" s="52">
+        <v>0</v>
+      </c>
+      <c r="AV179" s="52">
+        <v>0</v>
+      </c>
+      <c r="AW179" s="38">
+        <v>0</v>
+      </c>
+      <c r="AX179" s="38">
+        <v>0</v>
+      </c>
+      <c r="AY179" s="38">
+        <v>0</v>
+      </c>
+      <c r="AZ179" s="38">
+        <v>0</v>
+      </c>
+      <c r="BA179" s="38">
+        <v>0</v>
+      </c>
+      <c r="BB179" s="38">
+        <v>0</v>
+      </c>
+      <c r="BC179" s="38">
+        <v>0</v>
+      </c>
+      <c r="BD179" s="38">
+        <v>0</v>
+      </c>
+      <c r="BE179" s="38">
+        <v>0</v>
+      </c>
+      <c r="BF179" s="38">
+        <v>0</v>
+      </c>
+      <c r="BG179" s="40">
+        <v>1</v>
+      </c>
+      <c r="BH179" s="40" t="s">
+        <v>1416</v>
+      </c>
+      <c r="BI179" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A180" s="6">
+        <v>179</v>
+      </c>
+      <c r="B180" s="6" t="s">
+        <v>1617</v>
+      </c>
+      <c r="C180" s="6" t="s">
+        <v>1617</v>
+      </c>
+      <c r="D180" s="6" t="s">
+        <v>1618</v>
+      </c>
+      <c r="E180" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F180" s="17">
+        <v>45041.510416666664</v>
+      </c>
+      <c r="G180" s="21">
+        <v>2</v>
+      </c>
+      <c r="H180" s="4">
+        <f t="shared" si="10"/>
+        <v>45041.59375</v>
+      </c>
+      <c r="I180" s="3">
+        <v>500</v>
+      </c>
+      <c r="J180" s="3">
+        <v>17000</v>
+      </c>
+      <c r="K180" s="3">
+        <f t="shared" si="13"/>
+        <v>1.7268164435946462E-2</v>
+      </c>
+      <c r="L180" s="3">
+        <v>153</v>
+      </c>
+      <c r="M180" s="3">
+        <v>5</v>
+      </c>
+      <c r="N180" s="3" t="s">
+        <v>1334</v>
+      </c>
+      <c r="O180" s="3">
+        <v>53.76</v>
+      </c>
+      <c r="P180" s="3">
+        <v>9.64</v>
+      </c>
+      <c r="Q180" s="3">
+        <v>18000</v>
+      </c>
+      <c r="R180" s="3">
+        <v>18000</v>
+      </c>
+      <c r="S180" s="3">
+        <v>5000</v>
+      </c>
+      <c r="T180" s="3">
+        <v>5</v>
+      </c>
+      <c r="U180" s="3">
+        <v>12000</v>
+      </c>
+      <c r="V180" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="W180" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="X180" s="3">
+        <v>3500</v>
+      </c>
+      <c r="Y180" s="3">
+        <v>60000</v>
+      </c>
+      <c r="Z180" s="3">
+        <v>60000</v>
+      </c>
+      <c r="AA180" s="5">
+        <v>5000</v>
+      </c>
+      <c r="AB180" s="5">
+        <v>2</v>
+      </c>
+      <c r="AC180" s="5">
+        <v>2</v>
+      </c>
+      <c r="AD180" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE180" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF180" s="5">
+        <v>3000</v>
+      </c>
+      <c r="AG180" s="5">
+        <v>-1.5</v>
+      </c>
+      <c r="AH180" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="AI180" s="45">
+        <v>0</v>
+      </c>
+      <c r="AJ180" s="45">
+        <v>0</v>
+      </c>
+      <c r="AK180" s="45">
+        <v>0</v>
+      </c>
+      <c r="AL180" s="23">
+        <v>0</v>
+      </c>
+      <c r="AM180" s="23">
+        <v>0</v>
+      </c>
+      <c r="AN180" s="23">
+        <v>0</v>
+      </c>
+      <c r="AO180" s="23">
+        <v>0</v>
+      </c>
+      <c r="AP180" s="23">
+        <v>0</v>
+      </c>
+      <c r="AQ180" s="23">
+        <v>0</v>
+      </c>
+      <c r="AR180" s="25">
+        <v>0</v>
+      </c>
+      <c r="AS180" s="54">
+        <v>0</v>
+      </c>
+      <c r="AT180" s="52">
+        <v>0</v>
+      </c>
+      <c r="AU180" s="52">
+        <v>0</v>
+      </c>
+      <c r="AV180" s="52">
+        <v>0</v>
+      </c>
+      <c r="AW180" s="38">
+        <v>0</v>
+      </c>
+      <c r="AX180" s="38">
+        <v>0</v>
+      </c>
+      <c r="AY180" s="38">
+        <v>0</v>
+      </c>
+      <c r="AZ180" s="38">
+        <v>0</v>
+      </c>
+      <c r="BA180" s="38">
+        <v>0</v>
+      </c>
+      <c r="BB180" s="38">
+        <v>0</v>
+      </c>
+      <c r="BC180" s="38">
+        <v>0</v>
+      </c>
+      <c r="BD180" s="38">
+        <v>0</v>
+      </c>
+      <c r="BE180" s="38">
+        <v>0</v>
+      </c>
+      <c r="BF180" s="38">
+        <v>0</v>
+      </c>
+      <c r="BG180" s="40">
+        <v>2</v>
+      </c>
+      <c r="BH180" s="40" t="s">
+        <v>1619</v>
+      </c>
+      <c r="BI180" s="40">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -36262,10 +37080,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EF8CB18-6EA0-4ACF-8EE2-9DD1689EBB8B}">
-  <dimension ref="J15:T34"/>
+  <dimension ref="C2:T111"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="M98" sqref="L98:M98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36275,7 +37093,75 @@
     <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="15" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>15830</v>
+      </c>
+    </row>
+    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>21500</v>
+      </c>
+    </row>
+    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>19500</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>13600</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>44832</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>49000</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>9800</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>14800</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>15200</v>
+      </c>
+    </row>
+    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>20200</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>28600</v>
+      </c>
+    </row>
+    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>19160</v>
+      </c>
       <c r="J15">
         <v>3</v>
       </c>
@@ -36284,7 +37170,10 @@
         <v>18.43494882292201</v>
       </c>
     </row>
-    <row r="16" spans="10:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>18614.2</v>
+      </c>
       <c r="J16">
         <v>4</v>
       </c>
@@ -36293,7 +37182,30 @@
         <v>14.036243467926479</v>
       </c>
     </row>
-    <row r="21" spans="10:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>30400</v>
+      </c>
+    </row>
+    <row r="18" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>7827</v>
+      </c>
+    </row>
+    <row r="19" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="20" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>19998</v>
+      </c>
+    </row>
+    <row r="21" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>17965</v>
+      </c>
       <c r="R21">
         <v>100000</v>
       </c>
@@ -36301,7 +37213,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="10:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>59700</v>
+      </c>
       <c r="R22">
         <v>30000</v>
       </c>
@@ -36309,19 +37224,28 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="23" spans="10:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>14065</v>
+      </c>
       <c r="R23">
         <f>R21*R22</f>
         <v>3000000000</v>
       </c>
     </row>
-    <row r="24" spans="10:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>15300</v>
+      </c>
       <c r="R24">
         <f>R23/1000000</f>
         <v>3000</v>
       </c>
     </row>
-    <row r="25" spans="10:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>20000</v>
+      </c>
       <c r="J25" t="s">
         <v>1457</v>
       </c>
@@ -36332,7 +37256,10 @@
         <v>1458</v>
       </c>
     </row>
-    <row r="26" spans="10:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>15800</v>
+      </c>
       <c r="J26" t="s">
         <v>1450</v>
       </c>
@@ -36343,7 +37270,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="10:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>13395</v>
+      </c>
       <c r="J27" t="s">
         <v>1451</v>
       </c>
@@ -36354,7 +37284,10 @@
         <v>1452</v>
       </c>
     </row>
-    <row r="28" spans="10:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>15000</v>
+      </c>
       <c r="J28" t="s">
         <v>180</v>
       </c>
@@ -36375,7 +37308,10 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="29" spans="10:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>20950</v>
+      </c>
       <c r="J29" t="s">
         <v>1456</v>
       </c>
@@ -36396,7 +37332,10 @@
         <v>1452</v>
       </c>
     </row>
-    <row r="30" spans="10:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>28300</v>
+      </c>
       <c r="J30" t="s">
         <v>1454</v>
       </c>
@@ -36425,7 +37364,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="10:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>20960</v>
+      </c>
       <c r="J31" t="s">
         <v>556</v>
       </c>
@@ -36442,7 +37384,10 @@
         <v>1.2949999999999999</v>
       </c>
     </row>
-    <row r="32" spans="10:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <v>20930</v>
+      </c>
       <c r="J32" t="s">
         <v>1460</v>
       </c>
@@ -36458,18 +37403,502 @@
         <v>10.000000591845426</v>
       </c>
     </row>
-    <row r="33" spans="11:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>14235</v>
+      </c>
       <c r="K33">
         <v>2.7000000000000001E-3</v>
       </c>
     </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>14500</v>
+      </c>
       <c r="K34">
         <v>3.7000000000000002E-3</v>
       </c>
     </row>
+    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>21272</v>
+      </c>
+    </row>
+    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>14720</v>
+      </c>
+    </row>
+    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>22500</v>
+      </c>
+    </row>
+    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>16900</v>
+      </c>
+    </row>
+    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>12760</v>
+      </c>
+    </row>
+    <row r="40" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>18050</v>
+      </c>
+    </row>
+    <row r="41" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>13800</v>
+      </c>
+    </row>
+    <row r="42" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>14900</v>
+      </c>
+    </row>
+    <row r="43" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>14680</v>
+      </c>
+    </row>
+    <row r="44" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <v>18210</v>
+      </c>
+    </row>
+    <row r="45" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>13750</v>
+      </c>
+    </row>
+    <row r="46" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <v>24200</v>
+      </c>
+    </row>
+    <row r="47" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>21890</v>
+      </c>
+    </row>
+    <row r="48" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <v>17100</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <v>20860</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>16944</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <v>31690</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <v>19080</v>
+      </c>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <v>23000</v>
+      </c>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <v>21530</v>
+      </c>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <v>17000</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <v>14880</v>
+      </c>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <v>14646</v>
+      </c>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C61">
+        <v>12500</v>
+      </c>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <v>17970</v>
+      </c>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <v>16550</v>
+      </c>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C64">
+        <v>20100</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C65">
+        <v>17400</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C66">
+        <v>17055</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C67">
+        <v>28072.8632</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C68">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C69">
+        <v>13710</v>
+      </c>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C70">
+        <v>26300</v>
+      </c>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C71">
+        <v>29400</v>
+      </c>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C72">
+        <v>13150</v>
+      </c>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C73">
+        <v>10600</v>
+      </c>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C74">
+        <v>23260</v>
+      </c>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C75">
+        <v>12900</v>
+      </c>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C76">
+        <v>24501</v>
+      </c>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C77">
+        <v>26620</v>
+      </c>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C78">
+        <v>13000</v>
+      </c>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C79">
+        <v>14650</v>
+      </c>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C80">
+        <v>24020</v>
+      </c>
+    </row>
+    <row r="81" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C81">
+        <v>18300</v>
+      </c>
+    </row>
+    <row r="82" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C82">
+        <v>18190</v>
+      </c>
+    </row>
+    <row r="83" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C83">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="84" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C84">
+        <v>12138</v>
+      </c>
+    </row>
+    <row r="85" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C85">
+        <v>13330</v>
+      </c>
+    </row>
+    <row r="86" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C86">
+        <v>13100</v>
+      </c>
+    </row>
+    <row r="87" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C87">
+        <v>14010</v>
+      </c>
+    </row>
+    <row r="88" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C88">
+        <v>14360</v>
+      </c>
+    </row>
+    <row r="89" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C89">
+        <v>12897.75</v>
+      </c>
+    </row>
+    <row r="90" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C90">
+        <v>12750</v>
+      </c>
+      <c r="F90" s="56" t="s">
+        <v>1607</v>
+      </c>
+      <c r="G90" s="56" t="s">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="91" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C91">
+        <v>17240</v>
+      </c>
+      <c r="F91">
+        <v>50</v>
+      </c>
+      <c r="G91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C92">
+        <v>22810</v>
+      </c>
+      <c r="F92">
+        <v>6015</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C93">
+        <v>24000</v>
+      </c>
+      <c r="F93">
+        <v>11980</v>
+      </c>
+      <c r="G93">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C94">
+        <v>21350</v>
+      </c>
+      <c r="F94">
+        <v>17945</v>
+      </c>
+      <c r="G94">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="95" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C95">
+        <v>27900</v>
+      </c>
+      <c r="F95">
+        <v>23910</v>
+      </c>
+      <c r="G95">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="96" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C96">
+        <v>15160</v>
+      </c>
+      <c r="F96">
+        <v>29875</v>
+      </c>
+      <c r="G96">
+        <v>13</v>
+      </c>
+      <c r="L96">
+        <v>5.65</v>
+      </c>
+      <c r="M96">
+        <v>291.5</v>
+      </c>
+    </row>
+    <row r="97" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C97">
+        <v>31858</v>
+      </c>
+      <c r="F97">
+        <v>35840</v>
+      </c>
+      <c r="G97">
+        <v>4</v>
+      </c>
+      <c r="L97">
+        <v>4.53</v>
+      </c>
+      <c r="M97">
+        <v>294.98</v>
+      </c>
+    </row>
+    <row r="98" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C98">
+        <v>14202</v>
+      </c>
+      <c r="F98">
+        <v>41805</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+      <c r="L98">
+        <f>AVERAGE(L96:L97)</f>
+        <v>5.09</v>
+      </c>
+      <c r="M98">
+        <f>AVERAGE(M96:M97)</f>
+        <v>293.24</v>
+      </c>
+    </row>
+    <row r="99" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C99">
+        <v>12248</v>
+      </c>
+      <c r="F99">
+        <v>47770</v>
+      </c>
+      <c r="G99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C100">
+        <v>13640</v>
+      </c>
+      <c r="F100">
+        <v>53735</v>
+      </c>
+      <c r="G100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C101">
+        <v>16870</v>
+      </c>
+      <c r="F101" s="55" t="s">
+        <v>1608</v>
+      </c>
+      <c r="G101" s="55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C102">
+        <v>20500</v>
+      </c>
+    </row>
+    <row r="103" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C103">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="104" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C104">
+        <v>11882</v>
+      </c>
+    </row>
+    <row r="105" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C105">
+        <v>23218</v>
+      </c>
+    </row>
+    <row r="106" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C106">
+        <v>13851.53</v>
+      </c>
+    </row>
+    <row r="107" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C107">
+        <v>16440</v>
+      </c>
+    </row>
+    <row r="108" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C108">
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="109" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C109">
+        <v>14060.9</v>
+      </c>
+    </row>
+    <row r="110" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C110">
+        <v>14016</v>
+      </c>
+    </row>
+    <row r="111" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C111">
+        <v>17210</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -36478,7 +37907,7 @@
   <dimension ref="A7:V59"/>
   <sheetViews>
     <sheetView topLeftCell="D8" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36580,11 +38009,11 @@
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H11" s="16">
         <f>DEGREES(ATAN(J20/F15))</f>
-        <v>85.046742522157942</v>
+        <v>37.251854349444017</v>
       </c>
       <c r="J11">
         <f>90-H11</f>
-        <v>4.9532574778420582</v>
+        <v>52.748145650555983</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -36592,7 +38021,7 @@
         <v>89</v>
       </c>
       <c r="F12" s="15">
-        <v>13</v>
+        <v>88</v>
       </c>
       <c r="L12">
         <v>6.1</v>
@@ -36601,11 +38030,11 @@
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J13" s="16">
         <f>SQRT(F15^2+J20^2)</f>
-        <v>150.56227947264878</v>
+        <v>80.403786602373401</v>
       </c>
       <c r="L13">
         <f>J13/L12</f>
-        <v>24.682340897155541</v>
+        <v>13.180948623339903</v>
       </c>
       <c r="Q13" t="s">
         <v>404</v>
@@ -36623,13 +38052,13 @@
       </c>
       <c r="F15" s="16">
         <f>F12-F18</f>
-        <v>13</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M16">
         <f>90-H11</f>
-        <v>4.9532574778420582</v>
+        <v>52.748145650555983</v>
       </c>
     </row>
     <row r="18" spans="3:22" x14ac:dyDescent="0.25">
@@ -36637,7 +38066,7 @@
         <v>88</v>
       </c>
       <c r="F18" s="15">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="U18">
         <v>43</v>
@@ -36659,14 +38088,14 @@
         <v>85</v>
       </c>
       <c r="J20" s="15">
-        <v>150</v>
+        <v>48.67</v>
       </c>
       <c r="K20">
         <v>52</v>
       </c>
       <c r="N20">
         <f>8/COS(RADIANS(H11))</f>
-        <v>92.653710444706945</v>
+        <v>10.050473325296675</v>
       </c>
       <c r="U20">
         <f>U18/U19</f>
@@ -42869,10 +44298,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19EF0D29-302D-4894-9471-C390103E7AFC}">
-  <dimension ref="A1:D136"/>
+  <dimension ref="A1:D137"/>
   <sheetViews>
-    <sheetView topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="A136" sqref="A136"/>
+    <sheetView topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44365,6 +45794,17 @@
       </c>
       <c r="B136" s="32" t="s">
         <v>1575</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="33">
+        <v>140</v>
+      </c>
+      <c r="B137" s="32" t="s">
+        <v>1613</v>
+      </c>
+      <c r="C137" s="31">
+        <v>45039</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Searched areas template, data permissions
</commit_message>
<xml_diff>
--- a/AllEventData.xlsx
+++ b/AllEventData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\GitHub\strewnlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6386739F-967A-4102-B73A-261D9686215C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16765CF4-25CC-4419-823A-65858C2B821B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C46C341C-A654-450D-9491-A8F495B2F4ED}"/>
   </bookViews>
@@ -8740,10 +8740,10 @@
   <dimension ref="A1:BI180"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C172" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="T174" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A181" sqref="A181"/>
+      <selection pane="bottomRight" activeCell="AG180" sqref="AG180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36910,14 +36910,14 @@
         <v>45041.59375</v>
       </c>
       <c r="I180" s="3">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="J180" s="3">
-        <v>17000</v>
+        <v>20500</v>
       </c>
       <c r="K180" s="3">
         <f t="shared" si="13"/>
-        <v>1.7268164435946462E-2</v>
+        <v>2.0088432122370936E-2</v>
       </c>
       <c r="L180" s="3">
         <v>153</v>
@@ -36929,10 +36929,10 @@
         <v>1334</v>
       </c>
       <c r="O180" s="3">
-        <v>53.76</v>
+        <v>53.772651000000003</v>
       </c>
       <c r="P180" s="3">
-        <v>9.64</v>
+        <v>9.6109229999999997</v>
       </c>
       <c r="Q180" s="3">
         <v>18000</v>
@@ -36965,7 +36965,7 @@
         <v>60000</v>
       </c>
       <c r="AA180" s="5">
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="AB180" s="5">
         <v>2</v>
@@ -36974,19 +36974,19 @@
         <v>2</v>
       </c>
       <c r="AD180" s="5">
-        <v>0</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="AE180" s="5">
-        <v>0</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="AF180" s="5">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="AG180" s="5">
-        <v>-1.5</v>
+        <v>-1</v>
       </c>
       <c r="AH180" s="5">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="AI180" s="45">
         <v>0</v>
@@ -37083,7 +37083,7 @@
   <dimension ref="C2:T111"/>
   <sheetViews>
     <sheetView topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="M98" sqref="L98:M98"/>
+      <selection activeCell="I85" sqref="H85:I85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37663,15 +37663,35 @@
       <c r="C83">
         <v>16000</v>
       </c>
+      <c r="H83">
+        <v>53.784500000000001</v>
+      </c>
+      <c r="I83">
+        <v>9.6201899999999991</v>
+      </c>
     </row>
     <row r="84" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C84">
         <v>12138</v>
       </c>
+      <c r="H84">
+        <v>53.769359999999999</v>
+      </c>
+      <c r="I84">
+        <v>9.6132980000000003</v>
+      </c>
     </row>
     <row r="85" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C85">
         <v>13330</v>
+      </c>
+      <c r="H85">
+        <f>H84-H83</f>
+        <v>-1.5140000000002374E-2</v>
+      </c>
+      <c r="I85">
+        <f>I84-I83</f>
+        <v>-6.891999999998788E-3</v>
       </c>
     </row>
     <row r="86" spans="3:13" x14ac:dyDescent="0.25">
@@ -38436,7 +38456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020F006F-09CB-4518-A6A0-B4628B5EF033}">
   <dimension ref="A1:D250"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A70" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Speed Error calc fix
</commit_message>
<xml_diff>
--- a/AllEventData.xlsx
+++ b/AllEventData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\GitHub\strewnlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34469144-E33C-4B26-9180-809D7417418A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E19762-C9F6-472F-9D6B-E56718EE0F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1755" yWindow="810" windowWidth="21600" windowHeight="11385" xr2:uid="{C46C341C-A654-450D-9491-A8F495B2F4ED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C46C341C-A654-450D-9491-A8F495B2F4ED}"/>
   </bookViews>
   <sheets>
     <sheet name="AllEventData" sheetId="1" r:id="rId1"/>
@@ -158,7 +158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2965" uniqueCount="1638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2975" uniqueCount="1643">
   <si>
     <t>UTC Date and Time</t>
   </si>
@@ -5073,6 +5073,21 @@
   </si>
   <si>
     <t>score</t>
+  </si>
+  <si>
+    <t>Languedoc</t>
+  </si>
+  <si>
+    <t>Tioga Astro</t>
+  </si>
+  <si>
+    <t>Presly</t>
+  </si>
+  <si>
+    <t>Fireball Recovery and InterPlanetary Observation Network (FRIPON), https://fireball.fripon.org/</t>
+  </si>
+  <si>
+    <t>Neuvy-sur-Barangeon</t>
   </si>
 </sst>
 </file>
@@ -14032,13 +14047,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{332638A7-5364-4539-88F3-B010BD503402}">
-  <dimension ref="A1:BI188"/>
+  <dimension ref="A1:BI189"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="G178" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="L188" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="H179" sqref="H179"/>
+      <selection pane="bottomRight" activeCell="V190" sqref="V190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38031,7 +38046,7 @@
         <v>8</v>
       </c>
       <c r="H153" s="4">
-        <f t="shared" ref="H153:H188" si="10">F153+G153/24</f>
+        <f t="shared" ref="H153:H189" si="10">F153+G153/24</f>
         <v>44924.61954861111</v>
       </c>
       <c r="I153" s="3">
@@ -42211,7 +42226,7 @@
         <v>20500</v>
       </c>
       <c r="K180" s="3">
-        <f t="shared" ref="K180:K188" si="14">I180*J180^2/2/4.184/10^12</f>
+        <f t="shared" ref="K180:K189" si="14">I180*J180^2/2/4.184/10^12</f>
         <v>2.511054015296367E-2</v>
       </c>
       <c r="L180" s="3">
@@ -43872,6 +43887,196 @@
         <v>1416</v>
       </c>
       <c r="BI188" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A189" s="6">
+        <v>188</v>
+      </c>
+      <c r="B189" s="6" t="s">
+        <v>1642</v>
+      </c>
+      <c r="C189" s="6" t="s">
+        <v>1640</v>
+      </c>
+      <c r="D189" s="6" t="s">
+        <v>1638</v>
+      </c>
+      <c r="E189" s="6" t="s">
+        <v>631</v>
+      </c>
+      <c r="F189" s="17">
+        <v>45178.926215277781</v>
+      </c>
+      <c r="G189" s="21">
+        <v>2</v>
+      </c>
+      <c r="H189" s="4">
+        <f t="shared" si="10"/>
+        <v>45179.009548611117</v>
+      </c>
+      <c r="I189" s="3">
+        <v>10</v>
+      </c>
+      <c r="J189" s="3">
+        <v>17000</v>
+      </c>
+      <c r="K189" s="3">
+        <f t="shared" si="14"/>
+        <v>3.4536328871892925E-4</v>
+      </c>
+      <c r="L189" s="3">
+        <v>2.4195000000000002</v>
+      </c>
+      <c r="M189" s="3">
+        <v>49.635599999999997</v>
+      </c>
+      <c r="N189" s="3" t="s">
+        <v>1334</v>
+      </c>
+      <c r="O189" s="3">
+        <v>47.332197999999998</v>
+      </c>
+      <c r="P189" s="3">
+        <v>2.2825120000000001</v>
+      </c>
+      <c r="Q189" s="3">
+        <v>22600</v>
+      </c>
+      <c r="R189" s="3">
+        <f>Q189</f>
+        <v>22600</v>
+      </c>
+      <c r="S189" s="3">
+        <v>3500</v>
+      </c>
+      <c r="T189" s="3">
+        <f>M189</f>
+        <v>49.635599999999997</v>
+      </c>
+      <c r="U189" s="3">
+        <f>R189</f>
+        <v>22600</v>
+      </c>
+      <c r="V189" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="W189" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="X189" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y189" s="3">
+        <v>60000</v>
+      </c>
+      <c r="Z189" s="3">
+        <v>60000</v>
+      </c>
+      <c r="AA189" s="5">
+        <v>800</v>
+      </c>
+      <c r="AB189" s="5">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="AC189" s="5">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="AD189" s="5">
+        <v>1.7420000000001323E-3</v>
+      </c>
+      <c r="AE189" s="5">
+        <v>1.9860000000000433E-3</v>
+      </c>
+      <c r="AF189" s="5">
+        <v>1000</v>
+      </c>
+      <c r="AG189" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AH189" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI189" s="45">
+        <v>0</v>
+      </c>
+      <c r="AJ189" s="45">
+        <v>0</v>
+      </c>
+      <c r="AK189" s="45">
+        <v>0</v>
+      </c>
+      <c r="AL189" s="23">
+        <v>0</v>
+      </c>
+      <c r="AM189" s="23">
+        <v>0</v>
+      </c>
+      <c r="AN189" s="23">
+        <v>0</v>
+      </c>
+      <c r="AO189" s="23">
+        <v>0</v>
+      </c>
+      <c r="AP189" s="23">
+        <v>0</v>
+      </c>
+      <c r="AQ189" s="23">
+        <v>0</v>
+      </c>
+      <c r="AR189" s="25">
+        <v>0</v>
+      </c>
+      <c r="AS189" s="54">
+        <v>0</v>
+      </c>
+      <c r="AT189" s="52">
+        <v>0</v>
+      </c>
+      <c r="AU189" s="52">
+        <v>0</v>
+      </c>
+      <c r="AV189" s="52">
+        <v>0</v>
+      </c>
+      <c r="AW189" s="38">
+        <v>0</v>
+      </c>
+      <c r="AX189" s="38">
+        <v>143</v>
+      </c>
+      <c r="AY189" s="38">
+        <v>0</v>
+      </c>
+      <c r="AZ189" s="38">
+        <v>0</v>
+      </c>
+      <c r="BA189" s="38">
+        <v>0</v>
+      </c>
+      <c r="BB189" s="38">
+        <v>0</v>
+      </c>
+      <c r="BC189" s="38">
+        <v>144</v>
+      </c>
+      <c r="BD189" s="38">
+        <v>0</v>
+      </c>
+      <c r="BE189" s="38">
+        <v>0</v>
+      </c>
+      <c r="BF189" s="38">
+        <v>0</v>
+      </c>
+      <c r="BG189" s="40">
+        <v>3</v>
+      </c>
+      <c r="BH189" s="40" t="s">
+        <v>1639</v>
+      </c>
+      <c r="BI189" s="40">
         <v>0</v>
       </c>
     </row>
@@ -44927,7 +45132,7 @@
   <dimension ref="A7:V59"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N11:N14"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45029,11 +45234,11 @@
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H11" s="16">
         <f>DEGREES(ATAN(J20/F15))</f>
-        <v>68.26615170741961</v>
+        <v>48.868761607215369</v>
       </c>
       <c r="J11">
         <f>90-H11</f>
-        <v>21.73384829258039</v>
+        <v>41.131238392784631</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -45041,20 +45246,20 @@
         <v>89</v>
       </c>
       <c r="F12" s="15">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="L12">
-        <v>6</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J13" s="16">
         <f>SQRT(F15^2+J20^2)</f>
-        <v>137.79532149169651</v>
+        <v>87.718498049157219</v>
       </c>
       <c r="L13">
         <f>J13/L12</f>
-        <v>22.965886915282752</v>
+        <v>13.923571118913845</v>
       </c>
       <c r="Q13" t="s">
         <v>404</v>
@@ -45072,13 +45277,13 @@
       </c>
       <c r="F15" s="16">
         <f>F12-F18</f>
-        <v>51.024999999999999</v>
+        <v>57.7</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M16">
         <f>90-H11</f>
-        <v>21.73384829258039</v>
+        <v>41.131238392784631</v>
       </c>
     </row>
     <row r="18" spans="3:22" x14ac:dyDescent="0.25">
@@ -45086,7 +45291,7 @@
         <v>88</v>
       </c>
       <c r="F18" s="15">
-        <v>26.975000000000001</v>
+        <v>22.3</v>
       </c>
       <c r="U18">
         <v>43</v>
@@ -45108,14 +45313,14 @@
         <v>85</v>
       </c>
       <c r="J20" s="15">
-        <v>128</v>
+        <v>66.069999999999993</v>
       </c>
       <c r="K20">
         <v>52</v>
       </c>
       <c r="N20">
         <f>8/COS(RADIANS(H11))</f>
-        <v>21.604362017316454</v>
+        <v>12.162010128132716</v>
       </c>
       <c r="U20">
         <f>U18/U19</f>
@@ -45460,7 +45665,7 @@
   <dimension ref="A1:D250"/>
   <sheetViews>
     <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50638,7 +50843,7 @@
         <v>2</v>
       </c>
       <c r="J107">
-        <f t="shared" ref="J106:J169" si="14">ABS(COS(RADIANS(2*I107)))+1</f>
+        <f t="shared" ref="J107:J169" si="14">ABS(COS(RADIANS(2*I107)))+1</f>
         <v>1.9975640502598242</v>
       </c>
     </row>
@@ -55398,10 +55603,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19EF0D29-302D-4894-9471-C390103E7AFC}">
-  <dimension ref="A1:D139"/>
+  <dimension ref="A1:D141"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B141" sqref="B141"/>
+    <sheetView topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="A141" sqref="A141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56926,6 +57131,25 @@
         <v>1487</v>
       </c>
     </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="33">
+        <v>143</v>
+      </c>
+      <c r="B140" s="32" t="s">
+        <v>1639</v>
+      </c>
+      <c r="C140" s="31">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="33">
+        <v>144</v>
+      </c>
+      <c r="B141" s="32" t="s">
+        <v>1641</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C1" xr:uid="{55C4805C-87A8-4D18-978D-FAFC0E5CA908}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C125">

</xml_diff>

<commit_message>
Timezone and Architecture Updates
created a reference data file and earth data file to load to globals at initialization
</commit_message>
<xml_diff>
--- a/AllEventData.xlsx
+++ b/AllEventData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\GitHub\strewnlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A717460-E724-4FAF-AF86-7F693F0CA08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F13BE29-7FB7-4F68-B49B-0FD5ACC8697B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C46C341C-A654-450D-9491-A8F495B2F4ED}"/>
   </bookViews>
@@ -222,7 +222,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4934" uniqueCount="1822">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4951" uniqueCount="1826">
   <si>
     <t>UTC Date and Time</t>
   </si>
@@ -5689,6 +5689,18 @@
   </si>
   <si>
     <t>Annie Morris</t>
+  </si>
+  <si>
+    <t>Mountain Home 40km</t>
+  </si>
+  <si>
+    <t>Mountain Home 50km</t>
+  </si>
+  <si>
+    <t>Mountain Home 30km</t>
+  </si>
+  <si>
+    <t>Annie Morris, AMS20</t>
   </si>
 </sst>
 </file>
@@ -14663,13 +14675,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{332638A7-5364-4539-88F3-B010BD503402}">
-  <dimension ref="A1:BI192"/>
+  <dimension ref="A1:BI194"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C173" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="V187" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B192" sqref="B192"/>
+      <selection pane="bottomRight" activeCell="AH192" sqref="AH192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45082,7 +45094,7 @@
         <v>191</v>
       </c>
       <c r="B192" s="6" t="s">
-        <v>1819</v>
+        <v>1824</v>
       </c>
       <c r="C192" s="6" t="s">
         <v>1819</v>
@@ -45107,43 +45119,43 @@
         <v>50</v>
       </c>
       <c r="J192" s="3">
-        <v>11970</v>
+        <v>12530</v>
       </c>
       <c r="K192" s="3">
         <f>I192*J192^2/2/4.184/10^12</f>
-        <v>8.5612392447418739E-4</v>
+        <v>9.381028919694072E-4</v>
       </c>
       <c r="L192" s="3">
-        <v>64.739999999999995</v>
+        <v>65.900000000000006</v>
       </c>
       <c r="M192" s="3">
-        <v>76.64</v>
+        <v>74.14</v>
       </c>
       <c r="N192" s="3" t="s">
         <v>1334</v>
       </c>
       <c r="O192" s="3">
-        <v>42.965649999999997</v>
+        <v>42.9636</v>
       </c>
       <c r="P192" s="3">
-        <v>-115.73570000000001</v>
+        <v>-115.6296</v>
       </c>
       <c r="Q192" s="3">
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="R192" s="3">
-        <v>40000</v>
+        <f>Q192</f>
+        <v>30000</v>
       </c>
       <c r="S192" s="3">
         <v>4000</v>
       </c>
       <c r="T192" s="3">
         <f>M192</f>
-        <v>76.64</v>
+        <v>74.14</v>
       </c>
       <c r="U192" s="3">
-        <f>Q192</f>
-        <v>40000</v>
+        <v>28000</v>
       </c>
       <c r="V192" s="3" t="s">
         <v>144</v>
@@ -45161,22 +45173,22 @@
         <v>60000</v>
       </c>
       <c r="AA192" s="5">
-        <v>1380</v>
+        <v>820</v>
       </c>
       <c r="AB192" s="5">
-        <v>1.23</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="AC192" s="5">
-        <v>2.96</v>
+        <v>0.46</v>
       </c>
       <c r="AD192" s="5">
-        <v>2.049999999997E-3</v>
+        <v>0</v>
       </c>
       <c r="AE192" s="5">
-        <v>0.106100000000012</v>
+        <v>0</v>
       </c>
       <c r="AF192" s="5">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="AG192" s="5">
         <v>-1</v>
@@ -45230,7 +45242,7 @@
         <v>0</v>
       </c>
       <c r="AX192" s="38">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AY192" s="38">
         <v>0</v>
@@ -45245,7 +45257,7 @@
         <v>0</v>
       </c>
       <c r="BC192" s="38">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="BD192" s="38">
         <v>0</v>
@@ -45263,6 +45275,380 @@
         <v>1821</v>
       </c>
       <c r="BI192" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A193" s="6">
+        <v>192</v>
+      </c>
+      <c r="B193" s="6" t="s">
+        <v>1822</v>
+      </c>
+      <c r="C193" s="6" t="s">
+        <v>1819</v>
+      </c>
+      <c r="D193" s="6" t="s">
+        <v>1820</v>
+      </c>
+      <c r="E193" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F193" s="17">
+        <v>45206.158368055556</v>
+      </c>
+      <c r="G193" s="21">
+        <v>-6</v>
+      </c>
+      <c r="H193" s="4">
+        <v>45205.908368055556</v>
+      </c>
+      <c r="I193" s="3">
+        <v>50</v>
+      </c>
+      <c r="J193" s="3">
+        <v>11910</v>
+      </c>
+      <c r="K193" s="3">
+        <v>8.5612392447418739E-4</v>
+      </c>
+      <c r="L193" s="3">
+        <v>64.855000000000004</v>
+      </c>
+      <c r="M193" s="3">
+        <v>76.349999999999994</v>
+      </c>
+      <c r="N193" s="3" t="s">
+        <v>1334</v>
+      </c>
+      <c r="O193" s="3">
+        <v>42.965699999999998</v>
+      </c>
+      <c r="P193" s="3">
+        <v>-115.7359</v>
+      </c>
+      <c r="Q193" s="3">
+        <v>40000</v>
+      </c>
+      <c r="R193" s="3">
+        <f>Q193</f>
+        <v>40000</v>
+      </c>
+      <c r="S193" s="3">
+        <v>4000</v>
+      </c>
+      <c r="T193" s="3">
+        <f t="shared" ref="T193:T194" si="0">M193</f>
+        <v>76.349999999999994</v>
+      </c>
+      <c r="U193" s="3">
+        <v>38000</v>
+      </c>
+      <c r="V193" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="W193" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="X193" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y193" s="3">
+        <v>60000</v>
+      </c>
+      <c r="Z193" s="3">
+        <v>60000</v>
+      </c>
+      <c r="AA193" s="5">
+        <v>790</v>
+      </c>
+      <c r="AB193" s="5">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AC193" s="5">
+        <v>0.63</v>
+      </c>
+      <c r="AD193" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE193" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF193" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG193" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AH193" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI193" s="45">
+        <v>0</v>
+      </c>
+      <c r="AJ193" s="45">
+        <v>0</v>
+      </c>
+      <c r="AK193" s="45">
+        <v>0</v>
+      </c>
+      <c r="AL193" s="23">
+        <v>0</v>
+      </c>
+      <c r="AM193" s="23">
+        <v>0</v>
+      </c>
+      <c r="AN193" s="23">
+        <v>0</v>
+      </c>
+      <c r="AO193" s="23">
+        <v>0</v>
+      </c>
+      <c r="AP193" s="23">
+        <v>0</v>
+      </c>
+      <c r="AQ193" s="23">
+        <v>0</v>
+      </c>
+      <c r="AR193" s="25">
+        <v>0</v>
+      </c>
+      <c r="AS193" s="54">
+        <v>0</v>
+      </c>
+      <c r="AT193" s="52">
+        <v>0</v>
+      </c>
+      <c r="AU193" s="52">
+        <v>0</v>
+      </c>
+      <c r="AV193" s="52">
+        <v>0</v>
+      </c>
+      <c r="AW193" s="38">
+        <v>0</v>
+      </c>
+      <c r="AX193" s="38">
+        <v>145</v>
+      </c>
+      <c r="AY193" s="38">
+        <v>0</v>
+      </c>
+      <c r="AZ193" s="38">
+        <v>0</v>
+      </c>
+      <c r="BA193" s="38">
+        <v>0</v>
+      </c>
+      <c r="BB193" s="38">
+        <v>0</v>
+      </c>
+      <c r="BC193" s="38">
+        <v>145</v>
+      </c>
+      <c r="BD193" s="38">
+        <v>0</v>
+      </c>
+      <c r="BE193" s="38">
+        <v>0</v>
+      </c>
+      <c r="BF193" s="38">
+        <v>0</v>
+      </c>
+      <c r="BG193" s="40">
+        <v>2</v>
+      </c>
+      <c r="BH193" s="40" t="s">
+        <v>1821</v>
+      </c>
+      <c r="BI193" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A194" s="6">
+        <v>193</v>
+      </c>
+      <c r="B194" s="6" t="s">
+        <v>1823</v>
+      </c>
+      <c r="C194" s="6" t="s">
+        <v>1819</v>
+      </c>
+      <c r="D194" s="6" t="s">
+        <v>1820</v>
+      </c>
+      <c r="E194" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F194" s="17">
+        <v>45206.158368055556</v>
+      </c>
+      <c r="G194" s="21">
+        <v>-6</v>
+      </c>
+      <c r="H194" s="4">
+        <v>45205.908368055556</v>
+      </c>
+      <c r="I194" s="3">
+        <v>50</v>
+      </c>
+      <c r="J194" s="3">
+        <v>11380</v>
+      </c>
+      <c r="K194" s="3">
+        <v>8.5612392447418739E-4</v>
+      </c>
+      <c r="L194" s="3">
+        <v>63.734999999999999</v>
+      </c>
+      <c r="M194" s="3">
+        <v>78.78</v>
+      </c>
+      <c r="N194" s="3" t="s">
+        <v>1334</v>
+      </c>
+      <c r="O194" s="3">
+        <v>42.967700000000001</v>
+      </c>
+      <c r="P194" s="3">
+        <v>-115.84180000000001</v>
+      </c>
+      <c r="Q194" s="3">
+        <v>50000</v>
+      </c>
+      <c r="R194" s="3">
+        <f>Q194</f>
+        <v>50000</v>
+      </c>
+      <c r="S194" s="3">
+        <v>4000</v>
+      </c>
+      <c r="T194" s="3">
+        <f t="shared" si="0"/>
+        <v>78.78</v>
+      </c>
+      <c r="U194" s="3">
+        <v>48000</v>
+      </c>
+      <c r="V194" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="W194" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="X194" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y194" s="3">
+        <v>60000</v>
+      </c>
+      <c r="Z194" s="3">
+        <v>60000</v>
+      </c>
+      <c r="AA194" s="5">
+        <v>790</v>
+      </c>
+      <c r="AB194" s="5">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="AC194" s="5">
+        <v>0.82</v>
+      </c>
+      <c r="AD194" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE194" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF194" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG194" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AH194" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI194" s="45">
+        <v>0</v>
+      </c>
+      <c r="AJ194" s="45">
+        <v>0</v>
+      </c>
+      <c r="AK194" s="45">
+        <v>0</v>
+      </c>
+      <c r="AL194" s="23">
+        <v>0</v>
+      </c>
+      <c r="AM194" s="23">
+        <v>0</v>
+      </c>
+      <c r="AN194" s="23">
+        <v>0</v>
+      </c>
+      <c r="AO194" s="23">
+        <v>0</v>
+      </c>
+      <c r="AP194" s="23">
+        <v>0</v>
+      </c>
+      <c r="AQ194" s="23">
+        <v>0</v>
+      </c>
+      <c r="AR194" s="25">
+        <v>0</v>
+      </c>
+      <c r="AS194" s="54">
+        <v>0</v>
+      </c>
+      <c r="AT194" s="52">
+        <v>0</v>
+      </c>
+      <c r="AU194" s="52">
+        <v>0</v>
+      </c>
+      <c r="AV194" s="52">
+        <v>0</v>
+      </c>
+      <c r="AW194" s="38">
+        <v>0</v>
+      </c>
+      <c r="AX194" s="38">
+        <v>145</v>
+      </c>
+      <c r="AY194" s="38">
+        <v>0</v>
+      </c>
+      <c r="AZ194" s="38">
+        <v>0</v>
+      </c>
+      <c r="BA194" s="38">
+        <v>0</v>
+      </c>
+      <c r="BB194" s="38">
+        <v>0</v>
+      </c>
+      <c r="BC194" s="38">
+        <v>145</v>
+      </c>
+      <c r="BD194" s="38">
+        <v>0</v>
+      </c>
+      <c r="BE194" s="38">
+        <v>0</v>
+      </c>
+      <c r="BF194" s="38">
+        <v>0</v>
+      </c>
+      <c r="BG194" s="40">
+        <v>2</v>
+      </c>
+      <c r="BH194" s="40" t="s">
+        <v>1821</v>
+      </c>
+      <c r="BI194" s="40">
         <v>0</v>
       </c>
     </row>
@@ -87499,10 +87885,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19EF0D29-302D-4894-9471-C390103E7AFC}">
-  <dimension ref="A1:D141"/>
+  <dimension ref="A1:D142"/>
   <sheetViews>
     <sheetView topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="B152" sqref="B152"/>
+      <selection activeCell="B143" sqref="B143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -89046,6 +89432,14 @@
         <v>1640</v>
       </c>
     </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="33">
+        <v>145</v>
+      </c>
+      <c r="B142" s="32" t="s">
+        <v>1825</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C1" xr:uid="{55C4805C-87A8-4D18-978D-FAFC0E5CA908}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C125">

</xml_diff>

<commit_message>
Nearby sensor improvements, mailchimp fix
</commit_message>
<xml_diff>
--- a/AllEventData.xlsx
+++ b/AllEventData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\GitHub\strewnlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CD750C-B3BE-4F8D-B591-C0A92E425F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589CC892-91FB-4F48-B81B-6687EAB91022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32580" yWindow="1380" windowWidth="17280" windowHeight="11385" xr2:uid="{C46C341C-A654-450D-9491-A8F495B2F4ED}"/>
+    <workbookView xWindow="9735" yWindow="1245" windowWidth="21600" windowHeight="11385" xr2:uid="{C46C341C-A654-450D-9491-A8F495B2F4ED}"/>
   </bookViews>
   <sheets>
     <sheet name="AllEventData" sheetId="1" r:id="rId1"/>
@@ -224,7 +224,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5380" uniqueCount="2222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5380" uniqueCount="2223">
   <si>
     <t>UTC Date and Time</t>
   </si>
@@ -6891,6 +6891,9 @@
   </si>
   <si>
     <t>Quartzite</t>
+  </si>
+  <si>
+    <t>Emwaila</t>
   </si>
 </sst>
 </file>
@@ -15853,10 +15856,10 @@
   <dimension ref="A1:BI196"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="F191" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="N192" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="H194" sqref="H194"/>
+      <selection pane="bottomRight" activeCell="O196" sqref="O196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23631,11 +23634,11 @@
         <v>465681</v>
       </c>
       <c r="J62" s="3">
-        <v>17100</v>
+        <v>15861</v>
       </c>
       <c r="K62" s="3">
         <f t="shared" ref="K62:K72" si="4">I62*J62^2/2/4.184/10^12</f>
-        <v>16.272679398900571</v>
+        <v>13.99999812793989</v>
       </c>
       <c r="L62" s="3">
         <v>278.709</v>
@@ -23665,7 +23668,7 @@
         <v>85.509</v>
       </c>
       <c r="U62" s="3">
-        <v>15000</v>
+        <v>13000</v>
       </c>
       <c r="V62" s="3" t="s">
         <v>144</v>
@@ -23677,19 +23680,19 @@
         <v>0</v>
       </c>
       <c r="Y62" s="3">
-        <v>85000</v>
+        <v>60000</v>
       </c>
       <c r="Z62" s="3">
-        <v>85000</v>
+        <v>60000</v>
       </c>
       <c r="AA62" s="5">
         <v>500</v>
       </c>
       <c r="AB62" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AC62" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AD62" s="5">
         <v>0.05</v>
@@ -23701,10 +23704,10 @@
         <v>500</v>
       </c>
       <c r="AG62" s="5">
-        <v>-1.5</v>
+        <v>-1</v>
       </c>
       <c r="AH62" s="5">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="AI62" s="44" t="s">
         <v>1320</v>
@@ -23745,11 +23748,41 @@
       <c r="AV62" s="52">
         <v>0</v>
       </c>
-      <c r="BG62" s="40">
+      <c r="AW62" s="38">
+        <v>0</v>
+      </c>
+      <c r="AX62" s="38">
+        <v>0</v>
+      </c>
+      <c r="AY62" s="38">
+        <v>0</v>
+      </c>
+      <c r="AZ62" s="38">
+        <v>0</v>
+      </c>
+      <c r="BA62" s="38">
+        <v>0</v>
+      </c>
+      <c r="BB62" s="38">
+        <v>0</v>
+      </c>
+      <c r="BC62" s="38">
+        <v>4</v>
+      </c>
+      <c r="BD62" s="38">
+        <v>0</v>
+      </c>
+      <c r="BE62" s="38">
+        <v>0</v>
+      </c>
+      <c r="BF62" s="38">
+        <v>0</v>
+      </c>
+      <c r="BG62" s="41">
         <v>2</v>
       </c>
       <c r="BH62" s="40" t="s">
-        <v>1416</v>
+        <v>2222</v>
       </c>
       <c r="BI62" s="40">
         <v>0</v>
@@ -45755,7 +45788,7 @@
         <v>3500</v>
       </c>
       <c r="T189" s="3">
-        <f>M189</f>
+        <f t="shared" ref="T189:T196" si="15">M189</f>
         <v>53.131300000000003</v>
       </c>
       <c r="U189" s="3">
@@ -45945,7 +45978,7 @@
         <v>2500</v>
       </c>
       <c r="T190" s="3">
-        <f>M190</f>
+        <f t="shared" si="15"/>
         <v>36.557000000000002</v>
       </c>
       <c r="U190" s="3">
@@ -46135,7 +46168,7 @@
         <v>4100</v>
       </c>
       <c r="T191" s="3">
-        <f>M191</f>
+        <f t="shared" si="15"/>
         <v>64.163600000000002</v>
       </c>
       <c r="U191" s="3">
@@ -46325,7 +46358,7 @@
         <v>4000</v>
       </c>
       <c r="T192" s="3">
-        <f>M192</f>
+        <f t="shared" si="15"/>
         <v>74.14</v>
       </c>
       <c r="U192" s="3">
@@ -46513,7 +46546,7 @@
         <v>4000</v>
       </c>
       <c r="T193" s="3">
-        <f t="shared" ref="T193:T196" si="15">M193</f>
+        <f t="shared" si="15"/>
         <v>76.349999999999994</v>
       </c>
       <c r="U193" s="3">
@@ -46861,7 +46894,7 @@
         <v>71000</v>
       </c>
       <c r="K195" s="3">
-        <f t="shared" ref="K195:K196" si="16">I195*J195^2/2/4.184/10^12</f>
+        <f>I195*J195^2/2/4.184/10^12</f>
         <v>1.2048279158699809E-3</v>
       </c>
       <c r="L195" s="3">
@@ -47050,7 +47083,7 @@
         <v>13530</v>
       </c>
       <c r="K196" s="3">
-        <f t="shared" si="16"/>
+        <f>I196*J196^2/2/4.184/10^12</f>
         <v>2.1876302581261948E-3</v>
       </c>
       <c r="L196" s="3">
@@ -47063,10 +47096,10 @@
         <v>1334</v>
       </c>
       <c r="O196" s="3">
-        <v>33.876800000000003</v>
+        <v>33.882944999999999</v>
       </c>
       <c r="P196" s="3">
-        <v>-114.2052</v>
+        <v>-114.2671855</v>
       </c>
       <c r="Q196" s="3">
         <v>26206</v>
@@ -47087,7 +47120,7 @@
         <v>26206</v>
       </c>
       <c r="V196" s="3" t="s">
-        <v>144</v>
+        <v>81</v>
       </c>
       <c r="W196" s="3" t="s">
         <v>382</v>
@@ -47096,10 +47129,10 @@
         <v>0</v>
       </c>
       <c r="Y196" s="3">
-        <v>68000</v>
+        <v>60000</v>
       </c>
       <c r="Z196" s="3">
-        <v>68000</v>
+        <v>60000</v>
       </c>
       <c r="AA196" s="5">
         <v>283</v>
@@ -47108,13 +47141,13 @@
         <v>1</v>
       </c>
       <c r="AC196" s="5">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AD196" s="5">
-        <v>5.0000000000000001E-4</v>
+        <v>4.3140000000008172E-3</v>
       </c>
       <c r="AE196" s="5">
-        <v>5.0000000000000001E-4</v>
+        <v>1.2336500000003525E-2</v>
       </c>
       <c r="AF196" s="5">
         <v>1000</v>
@@ -47208,7 +47241,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A5:BI189" xr:uid="{332638A7-5364-4539-88F3-B010BD503402}"/>
+  <autoFilter ref="A5:BI189" xr:uid="{332638A7-5364-4539-88F3-B010BD503402}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:BI196">
+      <sortCondition ref="A5:A189"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -47219,7 +47256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19EF0D29-302D-4894-9471-C390103E7AFC}">
   <dimension ref="A1:D142"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B135" sqref="B135"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
GETWEATHER and configuration updates
</commit_message>
<xml_diff>
--- a/AllEventData.xlsx
+++ b/AllEventData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\GitHub\strewnlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84613A7B-F011-4ABF-A551-552CCC47F9CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC61E72-F1C9-4154-87EA-84B89693803C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C46C341C-A654-450D-9491-A8F495B2F4ED}"/>
   </bookViews>
@@ -224,7 +224,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5380" uniqueCount="2223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5388" uniqueCount="2226">
   <si>
     <t>UTC Date and Time</t>
   </si>
@@ -6894,6 +6894,15 @@
   </si>
   <si>
     <t>Emwaila</t>
+  </si>
+  <si>
+    <t>2024 BX1</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Rob Matson</t>
   </si>
 </sst>
 </file>
@@ -15853,13 +15862,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{332638A7-5364-4539-88F3-B010BD503402}">
-  <dimension ref="A1:BI196"/>
+  <dimension ref="A1:BI197"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C191" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="F194" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="J196" sqref="J196"/>
+      <selection pane="bottomRight" activeCell="H210" sqref="H210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39882,7 +39891,7 @@
         <v>8</v>
       </c>
       <c r="H153" s="4">
-        <f t="shared" ref="H153:H196" si="10">F153+G153/24</f>
+        <f t="shared" ref="H153:H197" si="10">F153+G153/24</f>
         <v>44924.61954861111</v>
       </c>
       <c r="I153" s="3">
@@ -45781,14 +45790,14 @@
         <v>22060.02</v>
       </c>
       <c r="R189" s="3">
-        <f t="shared" ref="R189:R196" si="14">Q189</f>
+        <f t="shared" ref="R189:R197" si="14">Q189</f>
         <v>22060.02</v>
       </c>
       <c r="S189" s="3">
         <v>3500</v>
       </c>
       <c r="T189" s="3">
-        <f t="shared" ref="T189:T196" si="15">M189</f>
+        <f t="shared" ref="T189:T197" si="15">M189</f>
         <v>53.131300000000003</v>
       </c>
       <c r="U189" s="3">
@@ -47237,6 +47246,196 @@
         <v>1416</v>
       </c>
       <c r="BI196" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A197" s="6">
+        <v>196</v>
+      </c>
+      <c r="B197" s="6" t="s">
+        <v>2223</v>
+      </c>
+      <c r="C197" s="6" t="s">
+        <v>2224</v>
+      </c>
+      <c r="D197" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="E197" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F197" s="17">
+        <v>45312.02270833333</v>
+      </c>
+      <c r="G197" s="21">
+        <v>1</v>
+      </c>
+      <c r="H197" s="4">
+        <f t="shared" si="10"/>
+        <v>45312.064374999994</v>
+      </c>
+      <c r="I197" s="3">
+        <v>1727</v>
+      </c>
+      <c r="J197" s="3">
+        <v>15221</v>
+      </c>
+      <c r="K197" s="3">
+        <f>I197*J197^2/2/4.184/10^12</f>
+        <v>4.7814215870817398E-2</v>
+      </c>
+      <c r="L197" s="3">
+        <v>74.063199999999995</v>
+      </c>
+      <c r="M197" s="3">
+        <v>14.5168</v>
+      </c>
+      <c r="N197" s="3" t="s">
+        <v>1334</v>
+      </c>
+      <c r="O197" s="3">
+        <v>52.633274290000003</v>
+      </c>
+      <c r="P197" s="3">
+        <v>12.638593859964788</v>
+      </c>
+      <c r="Q197" s="3">
+        <v>22000</v>
+      </c>
+      <c r="R197" s="3">
+        <f t="shared" si="14"/>
+        <v>22000</v>
+      </c>
+      <c r="S197" s="3">
+        <v>5000</v>
+      </c>
+      <c r="T197" s="3">
+        <f t="shared" si="15"/>
+        <v>14.5168</v>
+      </c>
+      <c r="U197" s="3">
+        <v>22000</v>
+      </c>
+      <c r="V197" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="W197" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="X197" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y197" s="3">
+        <v>60000</v>
+      </c>
+      <c r="Z197" s="3">
+        <v>60000</v>
+      </c>
+      <c r="AA197" s="5">
+        <v>24</v>
+      </c>
+      <c r="AB197" s="5">
+        <f>AC197*4.91</f>
+        <v>0.49100000000000005</v>
+      </c>
+      <c r="AC197" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="AD197" s="5">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="AE197" s="5">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="AF197" s="5">
+        <v>20</v>
+      </c>
+      <c r="AG197" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AH197" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI197" s="45">
+        <v>0</v>
+      </c>
+      <c r="AJ197" s="45">
+        <v>0</v>
+      </c>
+      <c r="AK197" s="45">
+        <v>0</v>
+      </c>
+      <c r="AL197" s="23">
+        <v>0</v>
+      </c>
+      <c r="AM197" s="23">
+        <v>0</v>
+      </c>
+      <c r="AN197" s="23">
+        <v>0</v>
+      </c>
+      <c r="AO197" s="23">
+        <v>0</v>
+      </c>
+      <c r="AP197" s="23">
+        <v>0</v>
+      </c>
+      <c r="AQ197" s="23">
+        <v>0</v>
+      </c>
+      <c r="AR197" s="25">
+        <v>0</v>
+      </c>
+      <c r="AS197" s="54">
+        <v>0</v>
+      </c>
+      <c r="AT197" s="52">
+        <v>0</v>
+      </c>
+      <c r="AU197" s="52">
+        <v>0</v>
+      </c>
+      <c r="AV197" s="52">
+        <v>0</v>
+      </c>
+      <c r="AW197" s="38">
+        <v>0</v>
+      </c>
+      <c r="AX197" s="38">
+        <v>0</v>
+      </c>
+      <c r="AY197" s="38">
+        <v>0</v>
+      </c>
+      <c r="AZ197" s="38">
+        <v>0</v>
+      </c>
+      <c r="BA197" s="38">
+        <v>0</v>
+      </c>
+      <c r="BB197" s="38">
+        <v>0</v>
+      </c>
+      <c r="BC197" s="38">
+        <v>4</v>
+      </c>
+      <c r="BD197" s="38">
+        <v>0</v>
+      </c>
+      <c r="BE197" s="38">
+        <v>0</v>
+      </c>
+      <c r="BF197" s="38">
+        <v>0</v>
+      </c>
+      <c r="BG197" s="40">
+        <v>3</v>
+      </c>
+      <c r="BH197" s="40" t="s">
+        <v>2225</v>
+      </c>
+      <c r="BI197" s="40">
         <v>0</v>
       </c>
     </row>
@@ -47256,8 +47455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19EF0D29-302D-4894-9471-C390103E7AFC}">
   <dimension ref="A1:D142"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B135" sqref="B135"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Sensor Database and Task Scheduler
Sensor database improvements, scoring
ANALYZENEARBY
IMPORTCONTACTS and IMPORTCAMERAS added to Task Scheduler
</commit_message>
<xml_diff>
--- a/AllEventData.xlsx
+++ b/AllEventData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\GitHub\strewnlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DAFBD2-92C0-42D2-8B0B-2CAA2F67C6B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E28C724C-0981-462C-B8F2-E60E25462474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C46C341C-A654-450D-9491-A8F495B2F4ED}"/>
   </bookViews>
@@ -29,7 +29,7 @@
     <externalReference r:id="rId12"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">AllEventData!$A$5:$BI$198</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">AllEventData!$A$5:$BI$200</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Database!$A$1:$H$39</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Sources!$A$1:$C$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Time Zones'!$A$1:$L$1</definedName>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3469" uniqueCount="2059">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3485" uniqueCount="2064">
   <si>
     <t>UTC Date and Time</t>
   </si>
@@ -6338,6 +6338,21 @@
   </si>
   <si>
     <t>Minsk</t>
+  </si>
+  <si>
+    <t>Nizwa</t>
+  </si>
+  <si>
+    <t>Ad Dakhiliyah</t>
+  </si>
+  <si>
+    <t>Mike Farmer</t>
+  </si>
+  <si>
+    <t>Federalsburg</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -15297,13 +15312,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{332638A7-5364-4539-88F3-B010BD503402}">
-  <dimension ref="A1:BI199"/>
+  <dimension ref="A1:BI201"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="50" workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C186" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A200" sqref="A200:XFD200"/>
+      <selection pane="bottomRight" activeCell="I201" sqref="I201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19825,10 +19840,10 @@
         <v>0</v>
       </c>
       <c r="AG28" s="10">
-        <v>-1.5</v>
+        <v>-1</v>
       </c>
       <c r="AH28" s="10">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="AI28" s="44" t="s">
         <v>1320</v>
@@ -39327,7 +39342,7 @@
         <v>8</v>
       </c>
       <c r="H153" s="4">
-        <f t="shared" ref="H153:H199" si="10">F153+G153/24</f>
+        <f t="shared" ref="H153:H201" si="10">F153+G153/24</f>
         <v>44924.61954861111</v>
       </c>
       <c r="I153" s="3">
@@ -46339,7 +46354,7 @@
         <v>71000</v>
       </c>
       <c r="K195" s="3">
-        <f>I195*J195^2/2/4.184/10^12</f>
+        <f t="shared" ref="K195:K201" si="16">I195*J195^2/2/4.184/10^12</f>
         <v>1.2048279158699809E-3</v>
       </c>
       <c r="L195" s="3">
@@ -46528,7 +46543,7 @@
         <v>13530</v>
       </c>
       <c r="K196" s="3">
-        <f>I196*J196^2/2/4.184/10^12</f>
+        <f t="shared" si="16"/>
         <v>2.1876302581261948E-3</v>
       </c>
       <c r="L196" s="3">
@@ -46718,7 +46733,7 @@
         <v>15221</v>
       </c>
       <c r="K197" s="3">
-        <f>I197*J197^2/2/4.184/10^12</f>
+        <f t="shared" si="16"/>
         <v>4.7814215870817398E-2</v>
       </c>
       <c r="L197" s="3">
@@ -46908,7 +46923,7 @@
         <v>17900</v>
       </c>
       <c r="K198" s="3">
-        <f>I198*J198^2/2/4.184/10^12</f>
+        <f t="shared" si="16"/>
         <v>3.8289913957934988E-5</v>
       </c>
       <c r="L198" s="3">
@@ -47098,7 +47113,7 @@
         <v>12430</v>
       </c>
       <c r="K199" s="3">
-        <f>I199*J199^2/2/4.184/10^12</f>
+        <f t="shared" si="16"/>
         <v>1.8463778680688336E-3</v>
       </c>
       <c r="L199" s="3">
@@ -47254,8 +47269,385 @@
         <v>1</v>
       </c>
     </row>
+    <row r="200" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A200" s="6">
+        <v>199</v>
+      </c>
+      <c r="B200" s="6" t="s">
+        <v>2059</v>
+      </c>
+      <c r="C200" s="6" t="s">
+        <v>2059</v>
+      </c>
+      <c r="D200" s="6" t="s">
+        <v>2060</v>
+      </c>
+      <c r="E200" s="6" t="s">
+        <v>898</v>
+      </c>
+      <c r="F200" s="17">
+        <v>45348.472928240742</v>
+      </c>
+      <c r="G200" s="21">
+        <v>4</v>
+      </c>
+      <c r="H200" s="4">
+        <f t="shared" si="10"/>
+        <v>45348.639594907407</v>
+      </c>
+      <c r="I200" s="3">
+        <v>2057</v>
+      </c>
+      <c r="J200" s="3">
+        <v>22998</v>
+      </c>
+      <c r="K200" s="3">
+        <f t="shared" si="16"/>
+        <v>0.13001479018021034</v>
+      </c>
+      <c r="L200" s="3">
+        <v>51.503</v>
+      </c>
+      <c r="M200" s="3">
+        <v>64.709000000000003</v>
+      </c>
+      <c r="N200" s="3" t="s">
+        <v>1270</v>
+      </c>
+      <c r="O200" s="3">
+        <v>22.9</v>
+      </c>
+      <c r="P200" s="3">
+        <v>57.4</v>
+      </c>
+      <c r="Q200" s="3">
+        <v>35900</v>
+      </c>
+      <c r="R200" s="3">
+        <f>Q200</f>
+        <v>35900</v>
+      </c>
+      <c r="S200" s="3">
+        <v>5000</v>
+      </c>
+      <c r="T200" s="3">
+        <f>M200</f>
+        <v>64.709000000000003</v>
+      </c>
+      <c r="U200" s="3">
+        <v>12000</v>
+      </c>
+      <c r="V200" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="W200" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="X200" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y200" s="3">
+        <v>60000</v>
+      </c>
+      <c r="Z200" s="3">
+        <v>60000</v>
+      </c>
+      <c r="AA200" s="5">
+        <v>500</v>
+      </c>
+      <c r="AB200" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="AC200" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="AD200" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="AE200" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="AF200" s="5">
+        <v>500</v>
+      </c>
+      <c r="AG200" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AH200" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI200" s="45">
+        <v>0</v>
+      </c>
+      <c r="AJ200" s="45">
+        <v>0</v>
+      </c>
+      <c r="AK200" s="45">
+        <v>0</v>
+      </c>
+      <c r="AL200" s="23">
+        <v>0</v>
+      </c>
+      <c r="AM200" s="23">
+        <v>0</v>
+      </c>
+      <c r="AN200" s="23">
+        <v>0</v>
+      </c>
+      <c r="AO200" s="23">
+        <v>0</v>
+      </c>
+      <c r="AP200" s="23">
+        <v>0</v>
+      </c>
+      <c r="AQ200" s="23">
+        <v>0</v>
+      </c>
+      <c r="AR200" s="25">
+        <v>0</v>
+      </c>
+      <c r="AS200" s="54">
+        <v>0</v>
+      </c>
+      <c r="AT200" s="52">
+        <v>0</v>
+      </c>
+      <c r="AU200" s="52">
+        <v>0</v>
+      </c>
+      <c r="AV200" s="52">
+        <v>0</v>
+      </c>
+      <c r="AW200" s="38">
+        <v>0</v>
+      </c>
+      <c r="AX200" s="38">
+        <v>4</v>
+      </c>
+      <c r="AY200" s="38">
+        <v>0</v>
+      </c>
+      <c r="AZ200" s="38">
+        <v>0</v>
+      </c>
+      <c r="BA200" s="38">
+        <v>0</v>
+      </c>
+      <c r="BB200" s="38">
+        <v>0</v>
+      </c>
+      <c r="BC200" s="38">
+        <v>4</v>
+      </c>
+      <c r="BD200" s="38">
+        <v>0</v>
+      </c>
+      <c r="BE200" s="38">
+        <v>0</v>
+      </c>
+      <c r="BF200" s="38">
+        <v>0</v>
+      </c>
+      <c r="BG200" s="40">
+        <v>2</v>
+      </c>
+      <c r="BH200" s="40" t="s">
+        <v>2061</v>
+      </c>
+      <c r="BI200" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A201" s="6">
+        <v>200</v>
+      </c>
+      <c r="B201" s="6" t="s">
+        <v>2062</v>
+      </c>
+      <c r="C201" s="6" t="s">
+        <v>2062</v>
+      </c>
+      <c r="D201" s="6" t="s">
+        <v>1481</v>
+      </c>
+      <c r="E201" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F201" s="17">
+        <v>45392.321851851855</v>
+      </c>
+      <c r="G201" s="21">
+        <v>-4</v>
+      </c>
+      <c r="H201" s="4">
+        <f t="shared" si="10"/>
+        <v>45392.155185185191</v>
+      </c>
+      <c r="I201" s="3">
+        <v>100</v>
+      </c>
+      <c r="J201" s="3">
+        <v>28000</v>
+      </c>
+      <c r="K201" s="3">
+        <f t="shared" si="16"/>
+        <v>9.3690248565965577E-3</v>
+      </c>
+      <c r="L201" s="3">
+        <v>225</v>
+      </c>
+      <c r="M201" s="3">
+        <v>52</v>
+      </c>
+      <c r="N201" s="3" t="s">
+        <v>1334</v>
+      </c>
+      <c r="O201" s="3">
+        <v>38.774949999999997</v>
+      </c>
+      <c r="P201" s="3">
+        <v>-75.766750000000002</v>
+      </c>
+      <c r="Q201" s="3">
+        <v>41000</v>
+      </c>
+      <c r="R201" s="3">
+        <f>Q201</f>
+        <v>41000</v>
+      </c>
+      <c r="S201" s="3">
+        <v>8000</v>
+      </c>
+      <c r="T201" s="3">
+        <v>52.47</v>
+      </c>
+      <c r="U201" s="3">
+        <v>41000</v>
+      </c>
+      <c r="V201" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="W201" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="X201" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y201" s="3">
+        <v>60000</v>
+      </c>
+      <c r="Z201" s="3">
+        <v>60000</v>
+      </c>
+      <c r="AA201" s="5">
+        <v>2000</v>
+      </c>
+      <c r="AB201" s="5">
+        <v>2</v>
+      </c>
+      <c r="AC201" s="5">
+        <v>3.15</v>
+      </c>
+      <c r="AD201" s="5">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="AE201" s="5">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="AF201" s="5">
+        <v>4000</v>
+      </c>
+      <c r="AG201" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AH201" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI201" s="45">
+        <v>0</v>
+      </c>
+      <c r="AJ201" s="45">
+        <v>0</v>
+      </c>
+      <c r="AK201" s="45">
+        <v>0</v>
+      </c>
+      <c r="AL201" s="23">
+        <v>0</v>
+      </c>
+      <c r="AM201" s="23">
+        <v>0</v>
+      </c>
+      <c r="AN201" s="23">
+        <v>0</v>
+      </c>
+      <c r="AO201" s="23">
+        <v>0</v>
+      </c>
+      <c r="AP201" s="23">
+        <v>0</v>
+      </c>
+      <c r="AQ201" s="23">
+        <v>0</v>
+      </c>
+      <c r="AR201" s="25">
+        <v>0</v>
+      </c>
+      <c r="AS201" s="54">
+        <v>0</v>
+      </c>
+      <c r="AT201" s="52">
+        <v>0</v>
+      </c>
+      <c r="AU201" s="52">
+        <v>0</v>
+      </c>
+      <c r="AV201" s="52">
+        <v>0</v>
+      </c>
+      <c r="AW201" s="38">
+        <v>0</v>
+      </c>
+      <c r="AX201" s="38">
+        <v>0</v>
+      </c>
+      <c r="AY201" s="38">
+        <v>0</v>
+      </c>
+      <c r="AZ201" s="38">
+        <v>0</v>
+      </c>
+      <c r="BA201" s="38">
+        <v>0</v>
+      </c>
+      <c r="BB201" s="38">
+        <v>0</v>
+      </c>
+      <c r="BC201" s="38">
+        <v>0</v>
+      </c>
+      <c r="BD201" s="38">
+        <v>0</v>
+      </c>
+      <c r="BE201" s="38">
+        <v>0</v>
+      </c>
+      <c r="BF201" s="38">
+        <v>0</v>
+      </c>
+      <c r="BG201" s="40">
+        <v>3</v>
+      </c>
+      <c r="BH201" s="40" t="s">
+        <v>2063</v>
+      </c>
+      <c r="BI201" s="40">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A5:BI198" xr:uid="{332638A7-5364-4539-88F3-B010BD503402}"/>
+  <autoFilter ref="A5:BI200" xr:uid="{332638A7-5364-4539-88F3-B010BD503402}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -47266,7 +47658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19EF0D29-302D-4894-9471-C390103E7AFC}">
   <dimension ref="A1:D142"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" workbookViewId="0">
+    <sheetView topLeftCell="A141" workbookViewId="0">
       <selection activeCell="B135" sqref="B135"/>
     </sheetView>
   </sheetViews>
@@ -49873,7 +50265,7 @@
   <dimension ref="A2:V59"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="Q22" sqref="Q19:Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49985,11 +50377,11 @@
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H11" s="16">
         <f>DEGREES(ATAN(J20/F15))</f>
-        <v>78.690067525979785</v>
+        <v>55.619655276155136</v>
       </c>
       <c r="J11">
         <f>90-H11</f>
-        <v>11.309932474020215</v>
+        <v>34.380344723844864</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -49997,20 +50389,17 @@
         <v>89</v>
       </c>
       <c r="F12" s="15">
-        <v>30</v>
-      </c>
-      <c r="L12">
-        <v>3.9</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J13" s="16">
         <f>SQRT(F15^2+J20^2)</f>
-        <v>152.97058540778355</v>
-      </c>
-      <c r="L13">
+        <v>69.06518659932803</v>
+      </c>
+      <c r="L13" t="e">
         <f>J13/L12</f>
-        <v>39.22322702763681</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="Q13" t="s">
         <v>404</v>
@@ -50028,13 +50417,13 @@
       </c>
       <c r="F15" s="16">
         <f>F12-F18</f>
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M16">
         <f>90-H11</f>
-        <v>11.309932474020215</v>
+        <v>34.380344723844864</v>
       </c>
     </row>
     <row r="18" spans="3:22" x14ac:dyDescent="0.25">
@@ -50042,7 +50431,7 @@
         <v>88</v>
       </c>
       <c r="F18" s="15">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="U18">
         <v>43</v>
@@ -50064,14 +50453,14 @@
         <v>85</v>
       </c>
       <c r="J20" s="15">
-        <v>150</v>
+        <v>57</v>
       </c>
       <c r="K20">
         <v>52</v>
       </c>
       <c r="N20">
         <f>8/COS(RADIANS(H11))</f>
-        <v>40.79215610874229</v>
+        <v>14.167217763964725</v>
       </c>
       <c r="U20">
         <f>U18/U19</f>
@@ -50085,9 +50474,6 @@
       <c r="K21">
         <v>66</v>
       </c>
-      <c r="P21">
-        <v>14.784000000000001</v>
-      </c>
     </row>
     <row r="22" spans="3:22" x14ac:dyDescent="0.25">
       <c r="J22">
@@ -50100,10 +50486,6 @@
       <c r="L22">
         <v>42.8</v>
       </c>
-      <c r="P22">
-        <f>P21*2</f>
-        <v>29.568000000000001</v>
-      </c>
     </row>
     <row r="23" spans="3:22" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
@@ -50155,10 +50537,6 @@
       </c>
       <c r="J27">
         <v>0.86</v>
-      </c>
-      <c r="Q27">
-        <f>1/1000</f>
-        <v>1E-3</v>
       </c>
     </row>
     <row r="28" spans="3:22" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AMS disable step 1
</commit_message>
<xml_diff>
--- a/AllEventData.xlsx
+++ b/AllEventData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\GitHub\strewnlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE34220-AC34-418F-ABB6-BBA3F76FF8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A0FC08-7D4A-457C-A6E9-A7904D0AC7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{C46C341C-A654-450D-9491-A8F495B2F4ED}"/>
+    <workbookView xWindow="11400" yWindow="195" windowWidth="16200" windowHeight="11385" xr2:uid="{C46C341C-A654-450D-9491-A8F495B2F4ED}"/>
   </bookViews>
   <sheets>
     <sheet name="AllEventData" sheetId="1" r:id="rId1"/>
@@ -114,21 +114,10 @@
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="5" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -170,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3554" uniqueCount="2072">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3562" uniqueCount="2073">
   <si>
     <t>UTC Date and Time</t>
   </si>
@@ -6387,6 +6376,9 @@
   </si>
   <si>
     <t>Cagayan</t>
+  </si>
+  <si>
+    <t>Coatesville</t>
   </si>
 </sst>
 </file>
@@ -16778,13 +16770,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{332638A7-5364-4539-88F3-B010BD503402}">
-  <dimension ref="A1:BI213"/>
+  <dimension ref="A1:BI214"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="I207" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="S210" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="J214" sqref="J214"/>
+      <selection pane="bottomRight" activeCell="V215" sqref="V215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45920,7 +45912,7 @@
         <v>2</v>
       </c>
       <c r="H185" s="4">
-        <f t="shared" ref="H185:H213" si="14">F185+G185/24</f>
+        <f t="shared" ref="H185:H214" si="14">F185+G185/24</f>
         <v>45103.948043981487</v>
       </c>
       <c r="I185" s="3">
@@ -46707,7 +46699,7 @@
         <v>22060.02</v>
       </c>
       <c r="R189" s="3">
-        <f t="shared" ref="R189:R213" si="15">Q189</f>
+        <f t="shared" ref="R189:R212" si="15">Q189</f>
         <v>22060.02</v>
       </c>
       <c r="S189" s="3">
@@ -47820,7 +47812,7 @@
         <v>71000</v>
       </c>
       <c r="K195" s="3">
-        <f t="shared" ref="K195:K213" si="17">I195*J195^2/2/4.184/10^12</f>
+        <f t="shared" ref="K195:K214" si="17">I195*J195^2/2/4.184/10^12</f>
         <v>1.2048279158699809E-3</v>
       </c>
       <c r="L195" s="3">
@@ -51380,6 +51372,195 @@
         <v>2043</v>
       </c>
       <c r="BI213" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A214" s="6">
+        <v>213</v>
+      </c>
+      <c r="B214" s="6" t="s">
+        <v>2072</v>
+      </c>
+      <c r="C214" s="6" t="s">
+        <v>2072</v>
+      </c>
+      <c r="D214" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E214" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F214" s="17">
+        <v>45636.37777777778</v>
+      </c>
+      <c r="G214" s="21">
+        <v>-5</v>
+      </c>
+      <c r="H214" s="4">
+        <f t="shared" si="14"/>
+        <v>45636.169444444444</v>
+      </c>
+      <c r="I214" s="3">
+        <v>1000</v>
+      </c>
+      <c r="J214" s="3">
+        <v>15000</v>
+      </c>
+      <c r="K214" s="3">
+        <f t="shared" si="17"/>
+        <v>2.6888145315487572E-2</v>
+      </c>
+      <c r="L214" s="3">
+        <v>160</v>
+      </c>
+      <c r="M214" s="3">
+        <v>10</v>
+      </c>
+      <c r="N214" s="3" t="s">
+        <v>1334</v>
+      </c>
+      <c r="O214" s="3">
+        <v>39.648752999999999</v>
+      </c>
+      <c r="P214" s="3">
+        <v>-86.701441000000003</v>
+      </c>
+      <c r="Q214" s="3">
+        <v>30000</v>
+      </c>
+      <c r="R214" s="3">
+        <f>Q214</f>
+        <v>30000</v>
+      </c>
+      <c r="S214" s="3">
+        <v>5000</v>
+      </c>
+      <c r="T214" s="3">
+        <f>M214</f>
+        <v>10</v>
+      </c>
+      <c r="U214" s="3">
+        <v>30000</v>
+      </c>
+      <c r="V214" s="3" t="s">
+        <v>1433</v>
+      </c>
+      <c r="W214" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="X214" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y214" s="3">
+        <v>60000</v>
+      </c>
+      <c r="Z214" s="3">
+        <v>60000</v>
+      </c>
+      <c r="AA214" s="5">
+        <v>1300</v>
+      </c>
+      <c r="AB214" s="5">
+        <v>2</v>
+      </c>
+      <c r="AC214" s="5">
+        <v>2</v>
+      </c>
+      <c r="AD214" s="5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AE214" s="5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AF214" s="5">
+        <v>500</v>
+      </c>
+      <c r="AG214" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AH214" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI214" s="45">
+        <v>0</v>
+      </c>
+      <c r="AJ214" s="45">
+        <v>0</v>
+      </c>
+      <c r="AK214" s="45">
+        <v>0</v>
+      </c>
+      <c r="AL214" s="23">
+        <v>0</v>
+      </c>
+      <c r="AM214" s="23">
+        <v>0</v>
+      </c>
+      <c r="AN214" s="23">
+        <v>0</v>
+      </c>
+      <c r="AO214" s="23">
+        <v>0</v>
+      </c>
+      <c r="AP214" s="23">
+        <v>0</v>
+      </c>
+      <c r="AQ214" s="23">
+        <v>0</v>
+      </c>
+      <c r="AR214" s="25">
+        <v>0</v>
+      </c>
+      <c r="AS214" s="53">
+        <v>0</v>
+      </c>
+      <c r="AT214" s="51">
+        <v>0</v>
+      </c>
+      <c r="AU214" s="51">
+        <v>0</v>
+      </c>
+      <c r="AV214" s="51">
+        <v>0</v>
+      </c>
+      <c r="AW214" s="38">
+        <v>0</v>
+      </c>
+      <c r="AX214" s="38">
+        <v>0</v>
+      </c>
+      <c r="AY214" s="38">
+        <v>0</v>
+      </c>
+      <c r="AZ214" s="38">
+        <v>0</v>
+      </c>
+      <c r="BA214" s="38">
+        <v>0</v>
+      </c>
+      <c r="BB214" s="38">
+        <v>0</v>
+      </c>
+      <c r="BC214" s="38">
+        <v>0</v>
+      </c>
+      <c r="BD214" s="38">
+        <v>0</v>
+      </c>
+      <c r="BE214" s="38">
+        <v>0</v>
+      </c>
+      <c r="BF214" s="38">
+        <v>0</v>
+      </c>
+      <c r="BG214" s="40">
+        <v>3</v>
+      </c>
+      <c r="BH214" s="40" t="s">
+        <v>2043</v>
+      </c>
+      <c r="BI214" s="40">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
NEXRAD functions and SETCONFIG
</commit_message>
<xml_diff>
--- a/AllEventData.xlsx
+++ b/AllEventData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\GitHub\strewnlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEB63A1-0B24-46C1-A7DC-B42CF8A5DC8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAEED379-D019-4E78-9D8F-1634618DA09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C46C341C-A654-450D-9491-A8F495B2F4ED}"/>
   </bookViews>
@@ -16,103 +16,105 @@
     <sheet name="AllEventData" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="13" r:id="rId2"/>
     <sheet name="Calculator" sheetId="2" r:id="rId3"/>
-    <sheet name="Time Zones" sheetId="12" r:id="rId4"/>
-    <sheet name="Countries" sheetId="5" r:id="rId5"/>
-    <sheet name="Cameras" sheetId="8" r:id="rId6"/>
-    <sheet name="DataQuality" sheetId="6" r:id="rId7"/>
-    <sheet name="Database" sheetId="7" r:id="rId8"/>
-    <sheet name="Sources" sheetId="4" r:id="rId9"/>
-    <sheet name="Log" sheetId="3" r:id="rId10"/>
+    <sheet name="Radar" sheetId="14" r:id="rId4"/>
+    <sheet name="Time Zones" sheetId="12" r:id="rId5"/>
+    <sheet name="Countries" sheetId="5" r:id="rId6"/>
+    <sheet name="Cameras" sheetId="8" r:id="rId7"/>
+    <sheet name="DataQuality" sheetId="6" r:id="rId8"/>
+    <sheet name="Database" sheetId="7" r:id="rId9"/>
+    <sheet name="Sources" sheetId="4" r:id="rId10"/>
+    <sheet name="Log" sheetId="3" r:id="rId11"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId11"/>
+    <externalReference r:id="rId12"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">AllEventData!$A$5:$BI$216</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Database!$A$1:$H$39</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Sources!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Time Zones'!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Database!$A$1:$H$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Radar!$D$6:$M$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Sources!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Time Zones'!$A$1:$L$1</definedName>
     <definedName name="solver_adj" localSheetId="0" hidden="1">AllEventData!$I$7</definedName>
     <definedName name="solver_adj" localSheetId="2" hidden="1">Calculator!$F$18</definedName>
-    <definedName name="solver_adj" localSheetId="5" hidden="1">Cameras!$P$72</definedName>
+    <definedName name="solver_adj" localSheetId="6" hidden="1">Cameras!$P$72</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
-    <definedName name="solver_cvg" localSheetId="5" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="6" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_drv" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
-    <definedName name="solver_itr" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
-    <definedName name="solver_mip" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
-    <definedName name="solver_mni" localSheetId="5" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="6" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
-    <definedName name="solver_mrt" localSheetId="5" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="6" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_msl" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_neg" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
-    <definedName name="solver_nod" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_num" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_num" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_nwt" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">AllEventData!$K$7</definedName>
     <definedName name="solver_opt" localSheetId="2" hidden="1">Calculator!$H$11</definedName>
-    <definedName name="solver_opt" localSheetId="5" hidden="1">Cameras!$O$77</definedName>
+    <definedName name="solver_opt" localSheetId="6" hidden="1">Cameras!$O$77</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
-    <definedName name="solver_pre" localSheetId="5" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="6" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_rbv" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rlx" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_rsd" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_scl" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="6" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
-    <definedName name="solver_ssz" localSheetId="5" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="6" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
-    <definedName name="solver_tim" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="6" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
-    <definedName name="solver_tol" localSheetId="5" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="6" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_typ" localSheetId="2" hidden="1">3</definedName>
-    <definedName name="solver_typ" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="6" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0.15001</definedName>
     <definedName name="solver_val" localSheetId="2" hidden="1">43.8</definedName>
-    <definedName name="solver_val" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
-    <definedName name="solver_ver" localSheetId="5" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="6" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -170,7 +172,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3581" uniqueCount="2074">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3631" uniqueCount="2093">
   <si>
     <t>UTC Date and Time</t>
   </si>
@@ -6393,6 +6395,63 @@
   </si>
   <si>
     <t>Westfield Center</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>vcp</t>
+  </si>
+  <si>
+    <t>precip</t>
+  </si>
+  <si>
+    <t>clear</t>
+  </si>
+  <si>
+    <t>Precip</t>
+  </si>
+  <si>
+    <t>Clear</t>
+  </si>
+  <si>
+    <t>pulse</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>same</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>transition</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>opmode</t>
+  </si>
+  <si>
+    <t>raw</t>
+  </si>
+  <si>
+    <t>St. Croix</t>
+  </si>
+  <si>
+    <t>Weston</t>
   </si>
 </sst>
 </file>
@@ -6617,7 +6676,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -6761,6 +6820,7 @@
     <xf numFmtId="169" fontId="3" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Accent1" xfId="5" builtinId="30"/>
@@ -16769,13 +16829,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{332638A7-5364-4539-88F3-B010BD503402}">
-  <dimension ref="A1:BI217"/>
+  <dimension ref="A1:BI218"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C211" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C216" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="BG217" sqref="BG217"/>
+      <selection pane="bottomRight" activeCell="AD219" sqref="AD219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45911,7 +45971,7 @@
         <v>2</v>
       </c>
       <c r="H185" s="4">
-        <f t="shared" ref="H185:H217" si="14">F185+G185/24</f>
+        <f t="shared" ref="H185:H218" si="14">F185+G185/24</f>
         <v>45103.948043981487</v>
       </c>
       <c r="I185" s="3">
@@ -47811,7 +47871,7 @@
         <v>71000</v>
       </c>
       <c r="K195" s="3">
-        <f t="shared" ref="K195:K217" si="17">I195*J195^2/2/4.184/10^12</f>
+        <f t="shared" ref="K195:K218" si="17">I195*J195^2/2/4.184/10^12</f>
         <v>1.2048279158699809E-3</v>
       </c>
       <c r="L195" s="3">
@@ -52131,6 +52191,196 @@
         <v>2072</v>
       </c>
       <c r="BI217" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A218" s="6">
+        <v>217</v>
+      </c>
+      <c r="B218" s="6" t="s">
+        <v>2091</v>
+      </c>
+      <c r="C218" s="6" t="s">
+        <v>2092</v>
+      </c>
+      <c r="D218" s="6" t="s">
+        <v>1585</v>
+      </c>
+      <c r="E218" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F218" s="17">
+        <v>45709.045335648145</v>
+      </c>
+      <c r="G218" s="21">
+        <v>-5</v>
+      </c>
+      <c r="H218" s="4">
+        <f t="shared" si="14"/>
+        <v>45708.837002314809</v>
+      </c>
+      <c r="I218" s="3">
+        <v>100</v>
+      </c>
+      <c r="J218" s="3">
+        <v>20000</v>
+      </c>
+      <c r="K218" s="3">
+        <f t="shared" si="17"/>
+        <v>4.7801147227533453E-3</v>
+      </c>
+      <c r="L218" s="3">
+        <v>289.2</v>
+      </c>
+      <c r="M218" s="3">
+        <v>43</v>
+      </c>
+      <c r="N218" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="O218" s="3">
+        <v>45.768917000000002</v>
+      </c>
+      <c r="P218" s="3">
+        <v>-67.926389999999998</v>
+      </c>
+      <c r="Q218" s="3">
+        <v>20000</v>
+      </c>
+      <c r="R218" s="3">
+        <f>Q218</f>
+        <v>20000</v>
+      </c>
+      <c r="S218" s="3">
+        <v>5000</v>
+      </c>
+      <c r="T218" s="3">
+        <f>M218</f>
+        <v>43</v>
+      </c>
+      <c r="U218" s="3">
+        <f>R218</f>
+        <v>20000</v>
+      </c>
+      <c r="V218" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="W218" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="X218" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y218" s="3">
+        <v>60000</v>
+      </c>
+      <c r="Z218" s="3">
+        <v>60000</v>
+      </c>
+      <c r="AA218" s="5">
+        <v>1000</v>
+      </c>
+      <c r="AB218" s="5">
+        <v>5</v>
+      </c>
+      <c r="AC218" s="5">
+        <v>10</v>
+      </c>
+      <c r="AD218" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE218" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF218" s="5">
+        <v>1000</v>
+      </c>
+      <c r="AG218" s="5">
+        <v>-1</v>
+      </c>
+      <c r="AH218" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI218" s="45">
+        <v>0</v>
+      </c>
+      <c r="AJ218" s="45">
+        <v>0</v>
+      </c>
+      <c r="AK218" s="45">
+        <v>0</v>
+      </c>
+      <c r="AL218" s="23">
+        <v>0</v>
+      </c>
+      <c r="AM218" s="23">
+        <v>0</v>
+      </c>
+      <c r="AN218" s="23">
+        <v>0</v>
+      </c>
+      <c r="AO218" s="23">
+        <v>0</v>
+      </c>
+      <c r="AP218" s="23">
+        <v>0</v>
+      </c>
+      <c r="AQ218" s="23">
+        <v>0</v>
+      </c>
+      <c r="AR218" s="25">
+        <v>0</v>
+      </c>
+      <c r="AS218" s="52">
+        <v>0</v>
+      </c>
+      <c r="AT218" s="50">
+        <v>0</v>
+      </c>
+      <c r="AU218" s="50">
+        <v>0</v>
+      </c>
+      <c r="AV218" s="50">
+        <v>0</v>
+      </c>
+      <c r="AW218" s="38">
+        <v>0</v>
+      </c>
+      <c r="AX218" s="38">
+        <v>0</v>
+      </c>
+      <c r="AY218" s="38">
+        <v>0</v>
+      </c>
+      <c r="AZ218" s="38">
+        <v>0</v>
+      </c>
+      <c r="BA218" s="38">
+        <v>0</v>
+      </c>
+      <c r="BB218" s="38">
+        <v>0</v>
+      </c>
+      <c r="BC218" s="38">
+        <v>0</v>
+      </c>
+      <c r="BD218" s="38">
+        <v>0</v>
+      </c>
+      <c r="BE218" s="38">
+        <v>0</v>
+      </c>
+      <c r="BF218" s="38">
+        <v>0</v>
+      </c>
+      <c r="BG218" s="40">
+        <v>1</v>
+      </c>
+      <c r="BH218" s="40" t="s">
+        <v>1411</v>
+      </c>
+      <c r="BI218" s="40">
         <v>0</v>
       </c>
     </row>
@@ -52143,6 +52393,1581 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19EF0D29-302D-4894-9471-C390103E7AFC}">
+  <dimension ref="A1:D143"/>
+  <sheetViews>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="A143" sqref="A143"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" style="33" customWidth="1"/>
+    <col min="2" max="2" width="191.42578125" style="32" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>218</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>167</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>224</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="33">
+        <v>1</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="C2" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="33">
+        <v>2</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="C3" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="33">
+        <v>3</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="C4" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="33">
+        <v>4</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="C5" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="33">
+        <v>5</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="C6" s="31">
+        <v>43812</v>
+      </c>
+      <c r="D6" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="33">
+        <v>6</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>377</v>
+      </c>
+      <c r="C7" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="33">
+        <v>7</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>370</v>
+      </c>
+      <c r="C8" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="33">
+        <v>8</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>364</v>
+      </c>
+      <c r="C9" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="33">
+        <v>9</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>349</v>
+      </c>
+      <c r="C10" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="33">
+        <v>10</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="C11" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="33">
+        <v>11</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>352</v>
+      </c>
+      <c r="C12" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="33">
+        <v>12</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>332</v>
+      </c>
+      <c r="C13" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="33">
+        <v>13</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>331</v>
+      </c>
+      <c r="C14" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="33">
+        <v>14</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="C15" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="33">
+        <v>15</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="C16" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="33">
+        <v>16</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="C17" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="33">
+        <v>17</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>277</v>
+      </c>
+      <c r="C18" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="33">
+        <v>18</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>310</v>
+      </c>
+      <c r="C19" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="33">
+        <v>19</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>311</v>
+      </c>
+      <c r="C20" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="33">
+        <v>20</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>356</v>
+      </c>
+      <c r="C21" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="33">
+        <v>21</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>271</v>
+      </c>
+      <c r="C22" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="33">
+        <v>22</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>270</v>
+      </c>
+      <c r="C23" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="33">
+        <v>23</v>
+      </c>
+      <c r="B24" s="32" t="s">
+        <v>329</v>
+      </c>
+      <c r="C24" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="33">
+        <v>24</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>285</v>
+      </c>
+      <c r="C25" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="33">
+        <v>25</v>
+      </c>
+      <c r="B26" s="32" t="s">
+        <v>287</v>
+      </c>
+      <c r="C26" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="33">
+        <v>26</v>
+      </c>
+      <c r="B27" s="32" t="s">
+        <v>320</v>
+      </c>
+      <c r="C27" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="33">
+        <v>27</v>
+      </c>
+      <c r="B28" s="32" t="s">
+        <v>308</v>
+      </c>
+      <c r="C28" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="33">
+        <v>28</v>
+      </c>
+      <c r="B29" s="32" t="s">
+        <v>309</v>
+      </c>
+      <c r="C29" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="33">
+        <v>29</v>
+      </c>
+      <c r="B30" s="32" t="s">
+        <v>354</v>
+      </c>
+      <c r="C30" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="33">
+        <v>30</v>
+      </c>
+      <c r="B31" s="32" t="s">
+        <v>351</v>
+      </c>
+      <c r="C31" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="33">
+        <v>32</v>
+      </c>
+      <c r="B32" s="32" t="s">
+        <v>265</v>
+      </c>
+      <c r="C32" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="33">
+        <v>33</v>
+      </c>
+      <c r="B33" s="32" t="s">
+        <v>360</v>
+      </c>
+      <c r="C33" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="33">
+        <v>34</v>
+      </c>
+      <c r="B34" s="32" t="s">
+        <v>359</v>
+      </c>
+      <c r="C34" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="33">
+        <v>35</v>
+      </c>
+      <c r="B35" s="32" t="s">
+        <v>318</v>
+      </c>
+      <c r="C35" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="33">
+        <v>36</v>
+      </c>
+      <c r="B36" s="32" t="s">
+        <v>278</v>
+      </c>
+      <c r="C36" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="33">
+        <v>37</v>
+      </c>
+      <c r="B37" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="C37" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="33">
+        <v>39</v>
+      </c>
+      <c r="B38" s="32" t="s">
+        <v>282</v>
+      </c>
+      <c r="C38" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="33">
+        <v>40</v>
+      </c>
+      <c r="B39" s="32" t="s">
+        <v>283</v>
+      </c>
+      <c r="C39" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A40" s="33">
+        <v>41</v>
+      </c>
+      <c r="B40" s="32" t="s">
+        <v>317</v>
+      </c>
+      <c r="C40" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="33">
+        <v>42</v>
+      </c>
+      <c r="B41" s="32" t="s">
+        <v>336</v>
+      </c>
+      <c r="C41" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="33">
+        <v>43</v>
+      </c>
+      <c r="B42" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="C42" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="33">
+        <v>44</v>
+      </c>
+      <c r="B43" s="32" t="s">
+        <v>376</v>
+      </c>
+      <c r="C43" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="33">
+        <v>45</v>
+      </c>
+      <c r="B44" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="C44" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="33">
+        <v>46</v>
+      </c>
+      <c r="B45" s="32" t="s">
+        <v>363</v>
+      </c>
+      <c r="C45" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="33">
+        <v>47</v>
+      </c>
+      <c r="B46" s="32" t="s">
+        <v>378</v>
+      </c>
+      <c r="C46" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="33">
+        <v>48</v>
+      </c>
+      <c r="B47" s="32" t="s">
+        <v>350</v>
+      </c>
+      <c r="C47" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="33">
+        <v>51</v>
+      </c>
+      <c r="B48" s="32" t="s">
+        <v>273</v>
+      </c>
+      <c r="C48" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="33">
+        <v>52</v>
+      </c>
+      <c r="B49" s="32" t="s">
+        <v>361</v>
+      </c>
+      <c r="C49" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="33">
+        <v>53</v>
+      </c>
+      <c r="B50" s="32" t="s">
+        <v>260</v>
+      </c>
+      <c r="C50" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="33">
+        <v>54</v>
+      </c>
+      <c r="B51" s="32" t="s">
+        <v>303</v>
+      </c>
+      <c r="C51" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="33">
+        <v>55</v>
+      </c>
+      <c r="B52" s="32" t="s">
+        <v>304</v>
+      </c>
+      <c r="C52" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="33">
+        <v>56</v>
+      </c>
+      <c r="B53" s="32" t="s">
+        <v>313</v>
+      </c>
+      <c r="C53" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="33">
+        <v>57</v>
+      </c>
+      <c r="B54" s="32" t="s">
+        <v>374</v>
+      </c>
+      <c r="C54" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="33">
+        <v>58</v>
+      </c>
+      <c r="B55" s="32" t="s">
+        <v>321</v>
+      </c>
+      <c r="C55" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="33">
+        <v>59</v>
+      </c>
+      <c r="B56" s="32" t="s">
+        <v>327</v>
+      </c>
+      <c r="C56" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="33">
+        <v>60</v>
+      </c>
+      <c r="B57" s="32" t="s">
+        <v>330</v>
+      </c>
+      <c r="C57" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="33">
+        <v>61</v>
+      </c>
+      <c r="B58" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="C58" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="33">
+        <v>62</v>
+      </c>
+      <c r="B59" s="32" t="s">
+        <v>369</v>
+      </c>
+      <c r="C59" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="33">
+        <v>63</v>
+      </c>
+      <c r="B60" s="32" t="s">
+        <v>324</v>
+      </c>
+      <c r="C60" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="33">
+        <v>64</v>
+      </c>
+      <c r="B61" s="32" t="s">
+        <v>314</v>
+      </c>
+      <c r="C61" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="33">
+        <v>65</v>
+      </c>
+      <c r="B62" s="32" t="s">
+        <v>316</v>
+      </c>
+      <c r="C62" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="33">
+        <v>66</v>
+      </c>
+      <c r="B63" s="32" t="s">
+        <v>300</v>
+      </c>
+      <c r="C63" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="33">
+        <v>67</v>
+      </c>
+      <c r="B64" s="32" t="s">
+        <v>307</v>
+      </c>
+      <c r="C64" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="33">
+        <v>68</v>
+      </c>
+      <c r="B65" s="32" t="s">
+        <v>262</v>
+      </c>
+      <c r="C65" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="33">
+        <v>69</v>
+      </c>
+      <c r="B66" s="32" t="s">
+        <v>328</v>
+      </c>
+      <c r="C66" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="33">
+        <v>70</v>
+      </c>
+      <c r="B67" s="32" t="s">
+        <v>338</v>
+      </c>
+      <c r="C67" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A68" s="33">
+        <v>71</v>
+      </c>
+      <c r="B68" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="C68" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="33">
+        <v>72</v>
+      </c>
+      <c r="B69" s="32" t="s">
+        <v>294</v>
+      </c>
+      <c r="C69" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="33">
+        <v>73</v>
+      </c>
+      <c r="B70" s="32" t="s">
+        <v>326</v>
+      </c>
+      <c r="C70" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="33">
+        <v>74</v>
+      </c>
+      <c r="B71" s="32" t="s">
+        <v>375</v>
+      </c>
+      <c r="C71" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="33">
+        <v>75</v>
+      </c>
+      <c r="B72" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="C72" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A73" s="33">
+        <v>76</v>
+      </c>
+      <c r="B73" s="32" t="s">
+        <v>343</v>
+      </c>
+      <c r="C73" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="33">
+        <v>77</v>
+      </c>
+      <c r="B74" s="32" t="s">
+        <v>325</v>
+      </c>
+      <c r="C74" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="33">
+        <v>78</v>
+      </c>
+      <c r="B75" s="32" t="s">
+        <v>365</v>
+      </c>
+      <c r="C75" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="33">
+        <v>79</v>
+      </c>
+      <c r="B76" s="32" t="s">
+        <v>334</v>
+      </c>
+      <c r="C76" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="33">
+        <v>80</v>
+      </c>
+      <c r="B77" s="32" t="s">
+        <v>319</v>
+      </c>
+      <c r="C77" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="33">
+        <v>81</v>
+      </c>
+      <c r="B78" s="32" t="s">
+        <v>358</v>
+      </c>
+      <c r="C78" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="33">
+        <v>82</v>
+      </c>
+      <c r="B79" s="32" t="s">
+        <v>373</v>
+      </c>
+      <c r="C79" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A80" s="33">
+        <v>83</v>
+      </c>
+      <c r="B80" s="32" t="s">
+        <v>341</v>
+      </c>
+      <c r="C80" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="33">
+        <v>84</v>
+      </c>
+      <c r="B81" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="C81" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="33">
+        <v>85</v>
+      </c>
+      <c r="B82" s="32" t="s">
+        <v>264</v>
+      </c>
+      <c r="C82" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="33">
+        <v>86</v>
+      </c>
+      <c r="B83" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="C83" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="33">
+        <v>87</v>
+      </c>
+      <c r="B84" s="32" t="s">
+        <v>269</v>
+      </c>
+      <c r="C84" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="33">
+        <v>88</v>
+      </c>
+      <c r="B85" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="C85" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="33">
+        <v>89</v>
+      </c>
+      <c r="B86" s="32" t="s">
+        <v>274</v>
+      </c>
+      <c r="C86" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="33">
+        <v>90</v>
+      </c>
+      <c r="B87" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="C87" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="33">
+        <v>91</v>
+      </c>
+      <c r="B88" s="32" t="s">
+        <v>284</v>
+      </c>
+      <c r="C88" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="33">
+        <v>92</v>
+      </c>
+      <c r="B89" s="32" t="s">
+        <v>286</v>
+      </c>
+      <c r="C89" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="33">
+        <v>93</v>
+      </c>
+      <c r="B90" s="32" t="s">
+        <v>288</v>
+      </c>
+      <c r="C90" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="33">
+        <v>94</v>
+      </c>
+      <c r="B91" s="32" t="s">
+        <v>289</v>
+      </c>
+      <c r="C91" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="33">
+        <v>95</v>
+      </c>
+      <c r="B92" s="32" t="s">
+        <v>290</v>
+      </c>
+      <c r="C92" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="33">
+        <v>96</v>
+      </c>
+      <c r="B93" s="32" t="s">
+        <v>291</v>
+      </c>
+      <c r="C93" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="33">
+        <v>97</v>
+      </c>
+      <c r="B94" s="32" t="s">
+        <v>292</v>
+      </c>
+      <c r="C94" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="33">
+        <v>98</v>
+      </c>
+      <c r="B95" s="32" t="s">
+        <v>293</v>
+      </c>
+      <c r="C95" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="33">
+        <v>99</v>
+      </c>
+      <c r="B96" s="32" t="s">
+        <v>295</v>
+      </c>
+      <c r="C96" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="33">
+        <v>100</v>
+      </c>
+      <c r="B97" s="32" t="s">
+        <v>296</v>
+      </c>
+      <c r="C97" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="33">
+        <v>101</v>
+      </c>
+      <c r="B98" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="C98" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="33">
+        <v>102</v>
+      </c>
+      <c r="B99" s="32" t="s">
+        <v>298</v>
+      </c>
+      <c r="C99" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="33">
+        <v>103</v>
+      </c>
+      <c r="B100" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="C100" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="33">
+        <v>104</v>
+      </c>
+      <c r="B101" s="32" t="s">
+        <v>301</v>
+      </c>
+      <c r="C101" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="33">
+        <v>105</v>
+      </c>
+      <c r="B102" s="32" t="s">
+        <v>302</v>
+      </c>
+      <c r="C102" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A103" s="33">
+        <v>106</v>
+      </c>
+      <c r="B103" s="32" t="s">
+        <v>305</v>
+      </c>
+      <c r="C103" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A104" s="33">
+        <v>107</v>
+      </c>
+      <c r="B104" s="32" t="s">
+        <v>306</v>
+      </c>
+      <c r="C104" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A105" s="33">
+        <v>108</v>
+      </c>
+      <c r="B105" s="32" t="s">
+        <v>312</v>
+      </c>
+      <c r="C105" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="33">
+        <v>109</v>
+      </c>
+      <c r="B106" s="32" t="s">
+        <v>315</v>
+      </c>
+      <c r="C106" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="33">
+        <v>110</v>
+      </c>
+      <c r="B107" s="32" t="s">
+        <v>333</v>
+      </c>
+      <c r="C107" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="33">
+        <v>111</v>
+      </c>
+      <c r="B108" s="32" t="s">
+        <v>335</v>
+      </c>
+      <c r="C108" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="33">
+        <v>112</v>
+      </c>
+      <c r="B109" s="32" t="s">
+        <v>337</v>
+      </c>
+      <c r="C109" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="33">
+        <v>113</v>
+      </c>
+      <c r="B110" s="32" t="s">
+        <v>339</v>
+      </c>
+      <c r="C110" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="33">
+        <v>114</v>
+      </c>
+      <c r="B111" s="32" t="s">
+        <v>340</v>
+      </c>
+      <c r="C111" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="33">
+        <v>115</v>
+      </c>
+      <c r="B112" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="C112" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="33">
+        <v>116</v>
+      </c>
+      <c r="B113" s="32" t="s">
+        <v>344</v>
+      </c>
+      <c r="C113" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="33">
+        <v>117</v>
+      </c>
+      <c r="B114" s="32" t="s">
+        <v>345</v>
+      </c>
+      <c r="C114" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="33">
+        <v>118</v>
+      </c>
+      <c r="B115" s="32" t="s">
+        <v>346</v>
+      </c>
+      <c r="C115" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A116" s="33">
+        <v>119</v>
+      </c>
+      <c r="B116" s="32" t="s">
+        <v>347</v>
+      </c>
+      <c r="C116" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="33">
+        <v>120</v>
+      </c>
+      <c r="B117" s="32" t="s">
+        <v>348</v>
+      </c>
+      <c r="C117" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A118" s="33">
+        <v>121</v>
+      </c>
+      <c r="B118" s="32" t="s">
+        <v>355</v>
+      </c>
+      <c r="C118" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="33">
+        <v>122</v>
+      </c>
+      <c r="B119" s="32" t="s">
+        <v>357</v>
+      </c>
+      <c r="C119" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="33">
+        <v>123</v>
+      </c>
+      <c r="B120" s="32" t="s">
+        <v>362</v>
+      </c>
+      <c r="C120" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="33">
+        <v>124</v>
+      </c>
+      <c r="B121" s="32" t="s">
+        <v>366</v>
+      </c>
+      <c r="C121" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="33">
+        <v>125</v>
+      </c>
+      <c r="B122" s="32" t="s">
+        <v>367</v>
+      </c>
+      <c r="C122" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="33">
+        <v>126</v>
+      </c>
+      <c r="B123" s="32" t="s">
+        <v>368</v>
+      </c>
+      <c r="C123" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A124" s="33">
+        <v>127</v>
+      </c>
+      <c r="B124" s="32" t="s">
+        <v>371</v>
+      </c>
+      <c r="C124" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="33">
+        <v>128</v>
+      </c>
+      <c r="B125" s="32" t="s">
+        <v>372</v>
+      </c>
+      <c r="C125" s="31">
+        <v>43812</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="33">
+        <v>129</v>
+      </c>
+      <c r="B126" s="32" t="s">
+        <v>402</v>
+      </c>
+      <c r="C126" s="31">
+        <v>43840</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="33">
+        <v>130</v>
+      </c>
+      <c r="B127" s="32" t="s">
+        <v>407</v>
+      </c>
+      <c r="C127" s="31">
+        <v>43840</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="33">
+        <v>131</v>
+      </c>
+      <c r="B128" s="32" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C128" s="31">
+        <v>43859</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="33">
+        <v>132</v>
+      </c>
+      <c r="B129" s="32" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C129" s="31">
+        <v>43863</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="33">
+        <v>133</v>
+      </c>
+      <c r="B130" s="32" t="s">
+        <v>1306</v>
+      </c>
+      <c r="C130" s="31">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="33">
+        <v>134</v>
+      </c>
+      <c r="B131" s="32" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="33">
+        <v>135</v>
+      </c>
+      <c r="B132" s="32" t="s">
+        <v>1481</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="33">
+        <v>136</v>
+      </c>
+      <c r="B133" s="32" t="s">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="33">
+        <v>137</v>
+      </c>
+      <c r="B134" s="32" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="33">
+        <v>138</v>
+      </c>
+      <c r="B135" s="32" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="33">
+        <v>139</v>
+      </c>
+      <c r="B136" s="32" t="s">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="33">
+        <v>140</v>
+      </c>
+      <c r="B137" s="32" t="s">
+        <v>1582</v>
+      </c>
+      <c r="C137" s="31">
+        <v>45039</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="33">
+        <v>141</v>
+      </c>
+      <c r="B138" s="32" t="s">
+        <v>1594</v>
+      </c>
+      <c r="C138" s="31">
+        <v>45126</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="33">
+        <v>142</v>
+      </c>
+      <c r="B139" s="32" t="s">
+        <v>1468</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="33">
+        <v>143</v>
+      </c>
+      <c r="B140" s="32" t="s">
+        <v>1614</v>
+      </c>
+      <c r="C140" s="31">
+        <v>45180</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="33">
+        <v>144</v>
+      </c>
+      <c r="B141" s="32" t="s">
+        <v>1615</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="33">
+        <v>145</v>
+      </c>
+      <c r="B142" s="32" t="s">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="33">
+        <v>146</v>
+      </c>
+      <c r="B143" s="32" t="s">
+        <v>2054</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C1" xr:uid="{55C4805C-87A8-4D18-978D-FAFC0E5CA908}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C125">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E59A1EA5-6E5D-46A3-AAE6-F062C7845542}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -53254,8 +55079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BBF5B9B-0F72-45F1-9ED5-2AE8EF041BE8}">
   <dimension ref="A2:V59"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView topLeftCell="D2" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53325,7 +55150,7 @@
       </c>
       <c r="M8">
         <f>J13/M7</f>
-        <v>11.624011659441138</v>
+        <v>9.736315922917921</v>
       </c>
       <c r="N8" t="s">
         <v>2041</v>
@@ -53381,11 +55206,11 @@
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="H11" s="16">
         <f>DEGREES(ATAN(J20/F15))</f>
-        <v>52.60819167278752</v>
+        <v>43.531199285614179</v>
       </c>
       <c r="J11">
         <f>90-H11</f>
-        <v>37.39180832721248</v>
+        <v>46.468800714385821</v>
       </c>
       <c r="N11">
         <v>18980</v>
@@ -53405,7 +55230,7 @@
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J13" s="16">
         <f>SQRT(F15^2+J20^2)</f>
-        <v>98.804099105249676</v>
+        <v>82.758685344802331</v>
       </c>
       <c r="L13" t="e">
         <f>J13/L12</f>
@@ -53441,7 +55266,7 @@
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M16">
         <f>90-H11</f>
-        <v>37.39180832721248</v>
+        <v>46.468800714385821</v>
       </c>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.25">
@@ -53457,11 +55282,11 @@
         <v>85</v>
       </c>
       <c r="J20" s="15">
-        <v>78.5</v>
+        <v>57</v>
       </c>
       <c r="N20">
         <f>8/COS(RADIANS(H11))</f>
-        <v>13.173879880699957</v>
+        <v>11.034491379306978</v>
       </c>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.25">
@@ -53723,6 +55548,401 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65BAD52C-2606-4AE3-8999-EF60C3E86497}">
+  <dimension ref="C2:M20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>2074</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2081</v>
+      </c>
+    </row>
+    <row r="3" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>2075</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>2077</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2089</v>
+      </c>
+      <c r="F6" t="s">
+        <v>122</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2082</v>
+      </c>
+      <c r="H6" t="s">
+        <v>2088</v>
+      </c>
+      <c r="I6" t="s">
+        <v>2084</v>
+      </c>
+      <c r="K6" t="s">
+        <v>2090</v>
+      </c>
+      <c r="M6" t="s">
+        <v>2087</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2076</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2074</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>2078</v>
+      </c>
+      <c r="I8">
+        <v>5</v>
+      </c>
+      <c r="J8">
+        <f>I8*60</f>
+        <v>300</v>
+      </c>
+      <c r="K8">
+        <v>301</v>
+      </c>
+      <c r="L8">
+        <f>J8-K8</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2074</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>2083</v>
+      </c>
+      <c r="H9" t="s">
+        <v>2078</v>
+      </c>
+      <c r="I9">
+        <v>4.2</v>
+      </c>
+      <c r="J9">
+        <f>I9*60</f>
+        <v>252</v>
+      </c>
+      <c r="K9">
+        <v>249</v>
+      </c>
+      <c r="L9">
+        <f>J9-K9</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>2085</v>
+      </c>
+      <c r="D10">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2074</v>
+      </c>
+      <c r="F10">
+        <v>13</v>
+      </c>
+      <c r="H10" t="s">
+        <v>2078</v>
+      </c>
+      <c r="I10">
+        <v>6</v>
+      </c>
+      <c r="J10">
+        <f>I10*60</f>
+        <v>360</v>
+      </c>
+      <c r="K10">
+        <v>359</v>
+      </c>
+      <c r="L10">
+        <f>J10-K10</f>
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2075</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11" t="s">
+        <v>2083</v>
+      </c>
+      <c r="H11" t="s">
+        <v>2079</v>
+      </c>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>32</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2075</v>
+      </c>
+      <c r="F12">
+        <v>19</v>
+      </c>
+      <c r="G12" t="s">
+        <v>2086</v>
+      </c>
+      <c r="H12" t="s">
+        <v>2079</v>
+      </c>
+      <c r="I12">
+        <v>10</v>
+      </c>
+      <c r="J12">
+        <f>I12*60</f>
+        <v>600</v>
+      </c>
+      <c r="K12">
+        <v>597</v>
+      </c>
+      <c r="L12">
+        <f>J12-K12</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>35</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2075</v>
+      </c>
+      <c r="F14">
+        <v>7</v>
+      </c>
+      <c r="G14" t="s">
+        <v>2086</v>
+      </c>
+      <c r="H14" t="s">
+        <v>2079</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>112</v>
+      </c>
+      <c r="H15" t="s">
+        <v>2078</v>
+      </c>
+      <c r="I15">
+        <v>5.6</v>
+      </c>
+      <c r="J15">
+        <f>I15*60</f>
+        <v>336</v>
+      </c>
+      <c r="K15">
+        <v>312</v>
+      </c>
+      <c r="L15">
+        <f>J15-K15</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>2085</v>
+      </c>
+      <c r="D16">
+        <v>121</v>
+      </c>
+      <c r="H16" t="s">
+        <v>2078</v>
+      </c>
+      <c r="I16">
+        <v>5.75</v>
+      </c>
+      <c r="J16">
+        <f>I16*60</f>
+        <v>345</v>
+      </c>
+      <c r="K16">
+        <v>352</v>
+      </c>
+      <c r="L16">
+        <f t="shared" ref="L16:L20" si="0">J16-K16</f>
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>211</v>
+      </c>
+      <c r="H17" t="s">
+        <v>2078</v>
+      </c>
+      <c r="I17">
+        <v>5</v>
+      </c>
+      <c r="J17">
+        <f>I17*60</f>
+        <v>300</v>
+      </c>
+      <c r="K17">
+        <v>301</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>212</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2074</v>
+      </c>
+      <c r="F18">
+        <v>4</v>
+      </c>
+      <c r="G18" t="s">
+        <v>2083</v>
+      </c>
+      <c r="H18" t="s">
+        <v>2078</v>
+      </c>
+      <c r="I18">
+        <v>4.75</v>
+      </c>
+      <c r="J18">
+        <f>I18*60</f>
+        <v>285</v>
+      </c>
+      <c r="K18">
+        <v>295</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>215</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2074</v>
+      </c>
+      <c r="F19">
+        <v>8</v>
+      </c>
+      <c r="H19" t="s">
+        <v>2078</v>
+      </c>
+      <c r="I19">
+        <v>6</v>
+      </c>
+      <c r="J19">
+        <f>I19*60</f>
+        <v>360</v>
+      </c>
+      <c r="K19">
+        <v>416</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>-56</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>2085</v>
+      </c>
+      <c r="D20" s="53">
+        <v>221</v>
+      </c>
+      <c r="E20" t="s">
+        <v>2074</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="H20" t="s">
+        <v>2078</v>
+      </c>
+      <c r="I20">
+        <v>6</v>
+      </c>
+      <c r="J20">
+        <f>I20*60</f>
+        <v>360</v>
+      </c>
+      <c r="K20">
+        <v>358</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="D6:M20" xr:uid="{65BAD52C-2606-4AE3-8999-EF60C3E86497}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D7:M20">
+      <sortCondition ref="D6:D20"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF4690B-ED60-431C-A6ED-A0B01298B5D9}">
   <dimension ref="A1:C207"/>
   <sheetViews>
@@ -56017,7 +58237,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020F006F-09CB-4518-A6A0-B4628B5EF033}">
   <dimension ref="A1:D250"/>
   <sheetViews>
@@ -59539,7 +61759,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E00CB2-4C03-4E08-A2A2-C2F4859B5A17}">
   <dimension ref="F5:W525"/>
   <sheetViews>
@@ -64972,7 +67192,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F0A5485-B526-4F4A-98E6-46596A9C7AC6}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -65037,7 +67257,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3642CC9A-E743-4191-A934-02A4E166F560}">
   <dimension ref="A1:I93"/>
   <sheetViews>
@@ -65956,1579 +68176,4 @@
   <autoFilter ref="A1:H39" xr:uid="{F141679E-852A-4834-84BB-BC1A666E0D12}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19EF0D29-302D-4894-9471-C390103E7AFC}">
-  <dimension ref="A1:D143"/>
-  <sheetViews>
-    <sheetView topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="A143" sqref="A143"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.7109375" style="33" customWidth="1"/>
-    <col min="2" max="2" width="191.42578125" style="32" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" style="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
-        <v>218</v>
-      </c>
-      <c r="B1" s="35" t="s">
-        <v>167</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>224</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33">
-        <v>1</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>223</v>
-      </c>
-      <c r="C2" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="33">
-        <v>2</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>219</v>
-      </c>
-      <c r="C3" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="33">
-        <v>3</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>220</v>
-      </c>
-      <c r="C4" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="33">
-        <v>4</v>
-      </c>
-      <c r="B5" s="32" t="s">
-        <v>221</v>
-      </c>
-      <c r="C5" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="33">
-        <v>5</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>222</v>
-      </c>
-      <c r="C6" s="31">
-        <v>43812</v>
-      </c>
-      <c r="D6" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="33">
-        <v>6</v>
-      </c>
-      <c r="B7" s="32" t="s">
-        <v>377</v>
-      </c>
-      <c r="C7" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="33">
-        <v>7</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>370</v>
-      </c>
-      <c r="C8" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="33">
-        <v>8</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>364</v>
-      </c>
-      <c r="C9" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="33">
-        <v>9</v>
-      </c>
-      <c r="B10" s="32" t="s">
-        <v>349</v>
-      </c>
-      <c r="C10" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="33">
-        <v>10</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>266</v>
-      </c>
-      <c r="C11" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="33">
-        <v>11</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>352</v>
-      </c>
-      <c r="C12" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="33">
-        <v>12</v>
-      </c>
-      <c r="B13" s="32" t="s">
-        <v>332</v>
-      </c>
-      <c r="C13" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="33">
-        <v>13</v>
-      </c>
-      <c r="B14" s="32" t="s">
-        <v>331</v>
-      </c>
-      <c r="C14" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="33">
-        <v>14</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>268</v>
-      </c>
-      <c r="C15" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="33">
-        <v>15</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>275</v>
-      </c>
-      <c r="C16" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="33">
-        <v>16</v>
-      </c>
-      <c r="B17" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="C17" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="33">
-        <v>17</v>
-      </c>
-      <c r="B18" s="32" t="s">
-        <v>277</v>
-      </c>
-      <c r="C18" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="33">
-        <v>18</v>
-      </c>
-      <c r="B19" s="32" t="s">
-        <v>310</v>
-      </c>
-      <c r="C19" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="33">
-        <v>19</v>
-      </c>
-      <c r="B20" s="32" t="s">
-        <v>311</v>
-      </c>
-      <c r="C20" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="33">
-        <v>20</v>
-      </c>
-      <c r="B21" s="32" t="s">
-        <v>356</v>
-      </c>
-      <c r="C21" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="33">
-        <v>21</v>
-      </c>
-      <c r="B22" s="32" t="s">
-        <v>271</v>
-      </c>
-      <c r="C22" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="33">
-        <v>22</v>
-      </c>
-      <c r="B23" s="32" t="s">
-        <v>270</v>
-      </c>
-      <c r="C23" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="33">
-        <v>23</v>
-      </c>
-      <c r="B24" s="32" t="s">
-        <v>329</v>
-      </c>
-      <c r="C24" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="33">
-        <v>24</v>
-      </c>
-      <c r="B25" s="32" t="s">
-        <v>285</v>
-      </c>
-      <c r="C25" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="33">
-        <v>25</v>
-      </c>
-      <c r="B26" s="32" t="s">
-        <v>287</v>
-      </c>
-      <c r="C26" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="33">
-        <v>26</v>
-      </c>
-      <c r="B27" s="32" t="s">
-        <v>320</v>
-      </c>
-      <c r="C27" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="33">
-        <v>27</v>
-      </c>
-      <c r="B28" s="32" t="s">
-        <v>308</v>
-      </c>
-      <c r="C28" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="33">
-        <v>28</v>
-      </c>
-      <c r="B29" s="32" t="s">
-        <v>309</v>
-      </c>
-      <c r="C29" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="33">
-        <v>29</v>
-      </c>
-      <c r="B30" s="32" t="s">
-        <v>354</v>
-      </c>
-      <c r="C30" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="33">
-        <v>30</v>
-      </c>
-      <c r="B31" s="32" t="s">
-        <v>351</v>
-      </c>
-      <c r="C31" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="33">
-        <v>32</v>
-      </c>
-      <c r="B32" s="32" t="s">
-        <v>265</v>
-      </c>
-      <c r="C32" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="33">
-        <v>33</v>
-      </c>
-      <c r="B33" s="32" t="s">
-        <v>360</v>
-      </c>
-      <c r="C33" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="33">
-        <v>34</v>
-      </c>
-      <c r="B34" s="32" t="s">
-        <v>359</v>
-      </c>
-      <c r="C34" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="33">
-        <v>35</v>
-      </c>
-      <c r="B35" s="32" t="s">
-        <v>318</v>
-      </c>
-      <c r="C35" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="33">
-        <v>36</v>
-      </c>
-      <c r="B36" s="32" t="s">
-        <v>278</v>
-      </c>
-      <c r="C36" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="33">
-        <v>37</v>
-      </c>
-      <c r="B37" s="32" t="s">
-        <v>276</v>
-      </c>
-      <c r="C37" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="33">
-        <v>39</v>
-      </c>
-      <c r="B38" s="32" t="s">
-        <v>282</v>
-      </c>
-      <c r="C38" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="33">
-        <v>40</v>
-      </c>
-      <c r="B39" s="32" t="s">
-        <v>283</v>
-      </c>
-      <c r="C39" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A40" s="33">
-        <v>41</v>
-      </c>
-      <c r="B40" s="32" t="s">
-        <v>317</v>
-      </c>
-      <c r="C40" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="33">
-        <v>42</v>
-      </c>
-      <c r="B41" s="32" t="s">
-        <v>336</v>
-      </c>
-      <c r="C41" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="33">
-        <v>43</v>
-      </c>
-      <c r="B42" s="32" t="s">
-        <v>279</v>
-      </c>
-      <c r="C42" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="33">
-        <v>44</v>
-      </c>
-      <c r="B43" s="32" t="s">
-        <v>376</v>
-      </c>
-      <c r="C43" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="33">
-        <v>45</v>
-      </c>
-      <c r="B44" s="32" t="s">
-        <v>280</v>
-      </c>
-      <c r="C44" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="33">
-        <v>46</v>
-      </c>
-      <c r="B45" s="32" t="s">
-        <v>363</v>
-      </c>
-      <c r="C45" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="33">
-        <v>47</v>
-      </c>
-      <c r="B46" s="32" t="s">
-        <v>378</v>
-      </c>
-      <c r="C46" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="33">
-        <v>48</v>
-      </c>
-      <c r="B47" s="32" t="s">
-        <v>350</v>
-      </c>
-      <c r="C47" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="33">
-        <v>51</v>
-      </c>
-      <c r="B48" s="32" t="s">
-        <v>273</v>
-      </c>
-      <c r="C48" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="33">
-        <v>52</v>
-      </c>
-      <c r="B49" s="32" t="s">
-        <v>361</v>
-      </c>
-      <c r="C49" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="33">
-        <v>53</v>
-      </c>
-      <c r="B50" s="32" t="s">
-        <v>260</v>
-      </c>
-      <c r="C50" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="33">
-        <v>54</v>
-      </c>
-      <c r="B51" s="32" t="s">
-        <v>303</v>
-      </c>
-      <c r="C51" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="33">
-        <v>55</v>
-      </c>
-      <c r="B52" s="32" t="s">
-        <v>304</v>
-      </c>
-      <c r="C52" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="33">
-        <v>56</v>
-      </c>
-      <c r="B53" s="32" t="s">
-        <v>313</v>
-      </c>
-      <c r="C53" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="33">
-        <v>57</v>
-      </c>
-      <c r="B54" s="32" t="s">
-        <v>374</v>
-      </c>
-      <c r="C54" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="33">
-        <v>58</v>
-      </c>
-      <c r="B55" s="32" t="s">
-        <v>321</v>
-      </c>
-      <c r="C55" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="33">
-        <v>59</v>
-      </c>
-      <c r="B56" s="32" t="s">
-        <v>327</v>
-      </c>
-      <c r="C56" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="33">
-        <v>60</v>
-      </c>
-      <c r="B57" s="32" t="s">
-        <v>330</v>
-      </c>
-      <c r="C57" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="33">
-        <v>61</v>
-      </c>
-      <c r="B58" s="32" t="s">
-        <v>263</v>
-      </c>
-      <c r="C58" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="33">
-        <v>62</v>
-      </c>
-      <c r="B59" s="32" t="s">
-        <v>369</v>
-      </c>
-      <c r="C59" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="33">
-        <v>63</v>
-      </c>
-      <c r="B60" s="32" t="s">
-        <v>324</v>
-      </c>
-      <c r="C60" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="33">
-        <v>64</v>
-      </c>
-      <c r="B61" s="32" t="s">
-        <v>314</v>
-      </c>
-      <c r="C61" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="33">
-        <v>65</v>
-      </c>
-      <c r="B62" s="32" t="s">
-        <v>316</v>
-      </c>
-      <c r="C62" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="33">
-        <v>66</v>
-      </c>
-      <c r="B63" s="32" t="s">
-        <v>300</v>
-      </c>
-      <c r="C63" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="33">
-        <v>67</v>
-      </c>
-      <c r="B64" s="32" t="s">
-        <v>307</v>
-      </c>
-      <c r="C64" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="33">
-        <v>68</v>
-      </c>
-      <c r="B65" s="32" t="s">
-        <v>262</v>
-      </c>
-      <c r="C65" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="33">
-        <v>69</v>
-      </c>
-      <c r="B66" s="32" t="s">
-        <v>328</v>
-      </c>
-      <c r="C66" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="33">
-        <v>70</v>
-      </c>
-      <c r="B67" s="32" t="s">
-        <v>338</v>
-      </c>
-      <c r="C67" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A68" s="33">
-        <v>71</v>
-      </c>
-      <c r="B68" s="32" t="s">
-        <v>323</v>
-      </c>
-      <c r="C68" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="33">
-        <v>72</v>
-      </c>
-      <c r="B69" s="32" t="s">
-        <v>294</v>
-      </c>
-      <c r="C69" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="33">
-        <v>73</v>
-      </c>
-      <c r="B70" s="32" t="s">
-        <v>326</v>
-      </c>
-      <c r="C70" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="33">
-        <v>74</v>
-      </c>
-      <c r="B71" s="32" t="s">
-        <v>375</v>
-      </c>
-      <c r="C71" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="33">
-        <v>75</v>
-      </c>
-      <c r="B72" s="32" t="s">
-        <v>322</v>
-      </c>
-      <c r="C72" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A73" s="33">
-        <v>76</v>
-      </c>
-      <c r="B73" s="32" t="s">
-        <v>343</v>
-      </c>
-      <c r="C73" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="33">
-        <v>77</v>
-      </c>
-      <c r="B74" s="32" t="s">
-        <v>325</v>
-      </c>
-      <c r="C74" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="33">
-        <v>78</v>
-      </c>
-      <c r="B75" s="32" t="s">
-        <v>365</v>
-      </c>
-      <c r="C75" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="33">
-        <v>79</v>
-      </c>
-      <c r="B76" s="32" t="s">
-        <v>334</v>
-      </c>
-      <c r="C76" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="33">
-        <v>80</v>
-      </c>
-      <c r="B77" s="32" t="s">
-        <v>319</v>
-      </c>
-      <c r="C77" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="33">
-        <v>81</v>
-      </c>
-      <c r="B78" s="32" t="s">
-        <v>358</v>
-      </c>
-      <c r="C78" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="33">
-        <v>82</v>
-      </c>
-      <c r="B79" s="32" t="s">
-        <v>373</v>
-      </c>
-      <c r="C79" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A80" s="33">
-        <v>83</v>
-      </c>
-      <c r="B80" s="32" t="s">
-        <v>341</v>
-      </c>
-      <c r="C80" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="33">
-        <v>84</v>
-      </c>
-      <c r="B81" s="32" t="s">
-        <v>261</v>
-      </c>
-      <c r="C81" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A82" s="33">
-        <v>85</v>
-      </c>
-      <c r="B82" s="32" t="s">
-        <v>264</v>
-      </c>
-      <c r="C82" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="33">
-        <v>86</v>
-      </c>
-      <c r="B83" s="32" t="s">
-        <v>267</v>
-      </c>
-      <c r="C83" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="33">
-        <v>87</v>
-      </c>
-      <c r="B84" s="32" t="s">
-        <v>269</v>
-      </c>
-      <c r="C84" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="33">
-        <v>88</v>
-      </c>
-      <c r="B85" s="32" t="s">
-        <v>272</v>
-      </c>
-      <c r="C85" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="33">
-        <v>89</v>
-      </c>
-      <c r="B86" s="32" t="s">
-        <v>274</v>
-      </c>
-      <c r="C86" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="33">
-        <v>90</v>
-      </c>
-      <c r="B87" s="32" t="s">
-        <v>281</v>
-      </c>
-      <c r="C87" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="33">
-        <v>91</v>
-      </c>
-      <c r="B88" s="32" t="s">
-        <v>284</v>
-      </c>
-      <c r="C88" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="33">
-        <v>92</v>
-      </c>
-      <c r="B89" s="32" t="s">
-        <v>286</v>
-      </c>
-      <c r="C89" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="33">
-        <v>93</v>
-      </c>
-      <c r="B90" s="32" t="s">
-        <v>288</v>
-      </c>
-      <c r="C90" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="33">
-        <v>94</v>
-      </c>
-      <c r="B91" s="32" t="s">
-        <v>289</v>
-      </c>
-      <c r="C91" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="33">
-        <v>95</v>
-      </c>
-      <c r="B92" s="32" t="s">
-        <v>290</v>
-      </c>
-      <c r="C92" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="33">
-        <v>96</v>
-      </c>
-      <c r="B93" s="32" t="s">
-        <v>291</v>
-      </c>
-      <c r="C93" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="33">
-        <v>97</v>
-      </c>
-      <c r="B94" s="32" t="s">
-        <v>292</v>
-      </c>
-      <c r="C94" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="33">
-        <v>98</v>
-      </c>
-      <c r="B95" s="32" t="s">
-        <v>293</v>
-      </c>
-      <c r="C95" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="33">
-        <v>99</v>
-      </c>
-      <c r="B96" s="32" t="s">
-        <v>295</v>
-      </c>
-      <c r="C96" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="33">
-        <v>100</v>
-      </c>
-      <c r="B97" s="32" t="s">
-        <v>296</v>
-      </c>
-      <c r="C97" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="33">
-        <v>101</v>
-      </c>
-      <c r="B98" s="32" t="s">
-        <v>297</v>
-      </c>
-      <c r="C98" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="33">
-        <v>102</v>
-      </c>
-      <c r="B99" s="32" t="s">
-        <v>298</v>
-      </c>
-      <c r="C99" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="33">
-        <v>103</v>
-      </c>
-      <c r="B100" s="32" t="s">
-        <v>299</v>
-      </c>
-      <c r="C100" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="33">
-        <v>104</v>
-      </c>
-      <c r="B101" s="32" t="s">
-        <v>301</v>
-      </c>
-      <c r="C101" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="33">
-        <v>105</v>
-      </c>
-      <c r="B102" s="32" t="s">
-        <v>302</v>
-      </c>
-      <c r="C102" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A103" s="33">
-        <v>106</v>
-      </c>
-      <c r="B103" s="32" t="s">
-        <v>305</v>
-      </c>
-      <c r="C103" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A104" s="33">
-        <v>107</v>
-      </c>
-      <c r="B104" s="32" t="s">
-        <v>306</v>
-      </c>
-      <c r="C104" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A105" s="33">
-        <v>108</v>
-      </c>
-      <c r="B105" s="32" t="s">
-        <v>312</v>
-      </c>
-      <c r="C105" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="33">
-        <v>109</v>
-      </c>
-      <c r="B106" s="32" t="s">
-        <v>315</v>
-      </c>
-      <c r="C106" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="33">
-        <v>110</v>
-      </c>
-      <c r="B107" s="32" t="s">
-        <v>333</v>
-      </c>
-      <c r="C107" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="33">
-        <v>111</v>
-      </c>
-      <c r="B108" s="32" t="s">
-        <v>335</v>
-      </c>
-      <c r="C108" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="33">
-        <v>112</v>
-      </c>
-      <c r="B109" s="32" t="s">
-        <v>337</v>
-      </c>
-      <c r="C109" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="33">
-        <v>113</v>
-      </c>
-      <c r="B110" s="32" t="s">
-        <v>339</v>
-      </c>
-      <c r="C110" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="33">
-        <v>114</v>
-      </c>
-      <c r="B111" s="32" t="s">
-        <v>340</v>
-      </c>
-      <c r="C111" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="33">
-        <v>115</v>
-      </c>
-      <c r="B112" s="32" t="s">
-        <v>342</v>
-      </c>
-      <c r="C112" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="33">
-        <v>116</v>
-      </c>
-      <c r="B113" s="32" t="s">
-        <v>344</v>
-      </c>
-      <c r="C113" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="33">
-        <v>117</v>
-      </c>
-      <c r="B114" s="32" t="s">
-        <v>345</v>
-      </c>
-      <c r="C114" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="33">
-        <v>118</v>
-      </c>
-      <c r="B115" s="32" t="s">
-        <v>346</v>
-      </c>
-      <c r="C115" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A116" s="33">
-        <v>119</v>
-      </c>
-      <c r="B116" s="32" t="s">
-        <v>347</v>
-      </c>
-      <c r="C116" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="33">
-        <v>120</v>
-      </c>
-      <c r="B117" s="32" t="s">
-        <v>348</v>
-      </c>
-      <c r="C117" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A118" s="33">
-        <v>121</v>
-      </c>
-      <c r="B118" s="32" t="s">
-        <v>355</v>
-      </c>
-      <c r="C118" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="33">
-        <v>122</v>
-      </c>
-      <c r="B119" s="32" t="s">
-        <v>357</v>
-      </c>
-      <c r="C119" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="33">
-        <v>123</v>
-      </c>
-      <c r="B120" s="32" t="s">
-        <v>362</v>
-      </c>
-      <c r="C120" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="33">
-        <v>124</v>
-      </c>
-      <c r="B121" s="32" t="s">
-        <v>366</v>
-      </c>
-      <c r="C121" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="33">
-        <v>125</v>
-      </c>
-      <c r="B122" s="32" t="s">
-        <v>367</v>
-      </c>
-      <c r="C122" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="33">
-        <v>126</v>
-      </c>
-      <c r="B123" s="32" t="s">
-        <v>368</v>
-      </c>
-      <c r="C123" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A124" s="33">
-        <v>127</v>
-      </c>
-      <c r="B124" s="32" t="s">
-        <v>371</v>
-      </c>
-      <c r="C124" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="33">
-        <v>128</v>
-      </c>
-      <c r="B125" s="32" t="s">
-        <v>372</v>
-      </c>
-      <c r="C125" s="31">
-        <v>43812</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="33">
-        <v>129</v>
-      </c>
-      <c r="B126" s="32" t="s">
-        <v>402</v>
-      </c>
-      <c r="C126" s="31">
-        <v>43840</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="33">
-        <v>130</v>
-      </c>
-      <c r="B127" s="32" t="s">
-        <v>407</v>
-      </c>
-      <c r="C127" s="31">
-        <v>43840</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="33">
-        <v>131</v>
-      </c>
-      <c r="B128" s="32" t="s">
-        <v>1161</v>
-      </c>
-      <c r="C128" s="31">
-        <v>43859</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="33">
-        <v>132</v>
-      </c>
-      <c r="B129" s="32" t="s">
-        <v>1163</v>
-      </c>
-      <c r="C129" s="31">
-        <v>43863</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="33">
-        <v>133</v>
-      </c>
-      <c r="B130" s="32" t="s">
-        <v>1306</v>
-      </c>
-      <c r="C130" s="31">
-        <v>43922</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="33">
-        <v>134</v>
-      </c>
-      <c r="B131" s="32" t="s">
-        <v>1419</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" s="33">
-        <v>135</v>
-      </c>
-      <c r="B132" s="32" t="s">
-        <v>1481</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="33">
-        <v>136</v>
-      </c>
-      <c r="B133" s="32" t="s">
-        <v>1523</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" s="33">
-        <v>137</v>
-      </c>
-      <c r="B134" s="32" t="s">
-        <v>1507</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" s="33">
-        <v>138</v>
-      </c>
-      <c r="B135" s="32" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" s="33">
-        <v>139</v>
-      </c>
-      <c r="B136" s="32" t="s">
-        <v>1556</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" s="33">
-        <v>140</v>
-      </c>
-      <c r="B137" s="32" t="s">
-        <v>1582</v>
-      </c>
-      <c r="C137" s="31">
-        <v>45039</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="33">
-        <v>141</v>
-      </c>
-      <c r="B138" s="32" t="s">
-        <v>1594</v>
-      </c>
-      <c r="C138" s="31">
-        <v>45126</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" s="33">
-        <v>142</v>
-      </c>
-      <c r="B139" s="32" t="s">
-        <v>1468</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" s="33">
-        <v>143</v>
-      </c>
-      <c r="B140" s="32" t="s">
-        <v>1614</v>
-      </c>
-      <c r="C140" s="31">
-        <v>45180</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" s="33">
-        <v>144</v>
-      </c>
-      <c r="B141" s="32" t="s">
-        <v>1615</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" s="33">
-        <v>145</v>
-      </c>
-      <c r="B142" s="32" t="s">
-        <v>1628</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" s="33">
-        <v>146</v>
-      </c>
-      <c r="B143" s="32" t="s">
-        <v>2054</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:C1" xr:uid="{55C4805C-87A8-4D18-978D-FAFC0E5CA908}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C125">
-      <sortCondition ref="A1"/>
-    </sortState>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>